<commit_message>
Nachzahlung Einkommensteuer für das Jahr 2020
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpreissl/Documents/Finance/Steuern/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpreissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1429F4-A3DA-8A4E-BF68-3A002752790D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC057AC2-54BC-C542-BC1C-635110884493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26900" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="303">
   <si>
     <t>Zusatzkrankenversicherung (Merkur)</t>
   </si>
@@ -693,9 +693,6 @@
     <t>Nachforderung wurde am 28.1.2021 überwiesen und am 22.02.2021 beglichen</t>
   </si>
   <si>
-    <t>Nachforderung wurde noch nicht offiziell bestätigt</t>
-  </si>
-  <si>
     <t>Legende</t>
   </si>
   <si>
@@ -912,16 +909,34 @@
     <t>Nachforderung Einkommenssteuer für 2019 von 1202€</t>
   </si>
   <si>
-    <t>Am 27.01.2021 wurden 1202€ überwiesen wegen Einkommensteuer-Nachforderung für das Jahr 2019. Das wird am 22.02.2021 fällig</t>
-  </si>
-  <si>
     <t>Stand 03.02.2021</t>
   </si>
   <si>
     <t>Vorauszahlung für Einkommensteuer im Jahr 2021 beträgt 2665€ (1.Q: 310€;  2.Q: 1022€;  3.Q: 666€;  4.Q: 667€)</t>
   </si>
   <si>
-    <t>Am 03.02.2021 wurden 1332€ überwiesen wegen Vorauszahlung für 1.Q (310€ fällig am 15.02.2021) und 2.Q (1022€ fällig am 17.05.2021).</t>
+    <t>Vorgehensweise für Zahlung ans Finanzamt</t>
+  </si>
+  <si>
+    <t>1) ING einloggen und auf Finanzamtszahlung klicken</t>
+  </si>
+  <si>
+    <t>2) Finanzamt Freistadt Rohrbach Urfahr (FA52) auswählen</t>
+  </si>
+  <si>
+    <t>3) Steuernummer 465301182 eintragen</t>
+  </si>
+  <si>
+    <t>4) Abgabenart wählen + Betrag eingeben</t>
+  </si>
+  <si>
+    <t>Nachforderung wurde am 29.3.2021 überwiesen</t>
+  </si>
+  <si>
+    <t>Stand 29.03.2021</t>
+  </si>
+  <si>
+    <t>Am 27.01.2021 wurden 1202€ überwiesen wegen Einkommensteuer-Nachforderung für das Jahr 2019. (fällig am 22.02.2021)</t>
   </si>
   <si>
     <r>
@@ -946,23 +961,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) reicht das, d.h nach dem 17.05.2021 sollte Kontostand auf 0€ sein. (eventuell ergeben sich Änderungen für die Nachforderung 2021, wenn ich bis dahin die Steuererklärung für 2020 gemacht habe)</t>
+      <t>) reicht das, d.h nach dem 17.05.2021 sollte Kontostand auf 0€ sein. (eventuell ergeben sich Änderungen für die Vorauszahlungen 2021, wenn ich bis dahin die Steuererklärung für 2020 gemacht habe)</t>
     </r>
   </si>
   <si>
-    <t>Vorgehensweise für Zahlung ans Finanzamt</t>
-  </si>
-  <si>
-    <t>1) ING einloggen und auf Finanzamtszahlung klicken</t>
-  </si>
-  <si>
-    <t>2) Finanzamt Freistadt Rohrbach Urfahr (FA52) auswählen</t>
-  </si>
-  <si>
-    <t>3) Steuernummer 465301182 eintragen</t>
-  </si>
-  <si>
-    <t>4) Abgabenart wählen + Betrag eingeben</t>
+    <t>Am 29.03.2021 wurden 1761€ überwiesen wegen Einkommensteuer-Nachforderung für das Jahr 2020. (fällig am 06.05.2021)</t>
+  </si>
+  <si>
+    <t>Am 03.02.2021 wurden 1332€ überwiesen (Buchungstag 05.02.2021) wegen Vorauszahlung für 2021 (Grundlage 2665€) für 1.Q (310€ fällig am 15.02.2021) und 2.Q (1022€ fällig am 17.05.2021).</t>
+  </si>
+  <si>
+    <t>Warten bis ich die neuen Quartalsberechnungen bekomme und anschließend sofort die komplette fehlende Jahressumme (310€ + 1022€= 1332€ für 2021 schon überwiesen) überweisen, damit  2021 erledigt ist</t>
+  </si>
+  <si>
+    <t>Die Änderungen für die Vorauszahlung 2021 ergibt 3124€ (vorher 2665) =&gt; ich habe noch keinen Bescheid über die neuen Quartalsberechnungen erhalten. 1.Q über 310€ mit dem alt berechneten 2665€ wurde am 15.02.2021 fällig</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1482,7 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1572,34 +1584,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="6" applyBorder="1"/>
     <xf numFmtId="168" fontId="13" fillId="3" borderId="3" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1638,30 +1623,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="169" fontId="10" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="11" applyBorder="1"/>
     <xf numFmtId="169" fontId="4" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="7" applyBorder="1"/>
     <xf numFmtId="176" fontId="4" fillId="8" borderId="9" xfId="7" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="4" fillId="9" borderId="9" xfId="8" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1676,6 +1643,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="169" fontId="17" fillId="3" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1685,7 +1682,24 @@
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
@@ -3649,10 +3663,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBECB8A-D6CD-CD47-9D68-71B2A5A5BDE3}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3667,598 +3681,598 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="92"/>
+      <c r="A1" s="147" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="148"/>
+      <c r="C1" s="149"/>
       <c r="E1" s="82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="94">
+      <c r="A2" s="84" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="85">
         <f>C6</f>
         <v>805</v>
       </c>
-      <c r="C2" s="95"/>
+      <c r="C2" s="86"/>
       <c r="E2" s="44"/>
       <c r="F2" s="82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="96" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" s="97">
+      <c r="A3" s="87" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="88">
         <f>C7</f>
         <v>-805</v>
       </c>
-      <c r="C3" s="95"/>
+      <c r="C3" s="86"/>
       <c r="E3" s="46"/>
       <c r="F3" s="82" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="98" t="s">
-        <v>224</v>
-      </c>
-      <c r="B4" s="99">
+      <c r="A4" s="89" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="90">
         <f>B2+B3</f>
         <v>0</v>
       </c>
-      <c r="C4" s="95"/>
+      <c r="C4" s="86"/>
       <c r="E4" s="38"/>
       <c r="F4" s="82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="100"/>
-      <c r="C5" s="95"/>
+      <c r="A5" s="91"/>
+      <c r="C5" s="86"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="92" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="93" t="s">
         <v>225</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="C6" s="94">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="103">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="96" t="s">
+      <c r="B7" s="95" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="104" t="s">
-        <v>228</v>
-      </c>
-      <c r="C7" s="105">
+      <c r="C7" s="96">
         <v>-805</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106"/>
-      <c r="B8" s="107" t="s">
+      <c r="A8" s="97"/>
+      <c r="B8" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="99">
         <f>C6+C7</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="147" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="148"/>
+      <c r="C11" s="149"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="101" t="s">
-        <v>230</v>
-      </c>
-      <c r="B12" s="109">
+      <c r="B12" s="100">
         <f>C18</f>
         <v>837</v>
       </c>
-      <c r="C12" s="95"/>
+      <c r="C12" s="86"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="84" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="101">
+        <v>740</v>
+      </c>
+      <c r="C13" s="86"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="87" t="s">
         <v>231</v>
       </c>
-      <c r="B13" s="110">
-        <v>740</v>
-      </c>
-      <c r="C13" s="95"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="B14" s="111">
+      <c r="B14" s="102">
         <f>C17</f>
         <v>-837</v>
       </c>
-      <c r="C14" s="95"/>
+      <c r="C14" s="86"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="98" t="s">
-        <v>233</v>
-      </c>
-      <c r="B15" s="112">
+      <c r="A15" s="89" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" s="103">
         <f>B13+B14</f>
         <v>-97</v>
       </c>
-      <c r="C15" s="113"/>
+      <c r="C15" s="104"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="100"/>
-      <c r="C16" s="95"/>
+      <c r="A16" s="91"/>
+      <c r="C16" s="86"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="96" t="s">
+      <c r="A17" s="87" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" s="95" t="s">
         <v>234</v>
       </c>
-      <c r="B17" s="104" t="s">
+      <c r="C17" s="105">
+        <v>-837</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="114">
-        <v>-837</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="101" t="s">
+      <c r="B18" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="B18" s="102" t="s">
+      <c r="C18" s="106">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="92" t="s">
         <v>237</v>
       </c>
-      <c r="C18" s="115">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="101" t="s">
+      <c r="B19" s="107" t="s">
         <v>238</v>
       </c>
-      <c r="B19" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="115">
+      <c r="C19" s="106">
         <v>-97</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="106"/>
-      <c r="B20" s="107" t="s">
+      <c r="A20" s="97"/>
+      <c r="B20" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="117">
+      <c r="C20" s="108">
         <f>SUM(C17:C19)</f>
         <v>-97</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="147" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="148"/>
+      <c r="C23" s="149"/>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="109" t="s">
         <v>240</v>
       </c>
-      <c r="B23" s="91"/>
-      <c r="C23" s="92"/>
-    </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="118" t="s">
-        <v>241</v>
-      </c>
-      <c r="B24" s="119">
+      <c r="B24" s="110">
         <f>C30+C32+C33+C34+C35</f>
         <v>769</v>
       </c>
-      <c r="C24" s="95"/>
+      <c r="C24" s="86"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="84" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="111">
+        <v>581</v>
+      </c>
+      <c r="C25" s="86"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="87" t="s">
         <v>242</v>
       </c>
-      <c r="B25" s="120">
-        <v>581</v>
-      </c>
-      <c r="C25" s="95"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="B26" s="121">
+      <c r="B26" s="112">
         <f>C29+C31</f>
         <v>-837</v>
       </c>
-      <c r="C26" s="95" t="s">
-        <v>244</v>
+      <c r="C26" s="86" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="98" t="s">
-        <v>233</v>
-      </c>
-      <c r="B27" s="122">
+      <c r="A27" s="89" t="s">
+        <v>232</v>
+      </c>
+      <c r="B27" s="113">
         <f>B25-B24</f>
         <v>-188</v>
       </c>
-      <c r="C27" s="95"/>
+      <c r="C27" s="86"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="100"/>
-      <c r="C28" s="95"/>
+      <c r="A28" s="91"/>
+      <c r="C28" s="86"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="96" t="s">
+      <c r="A29" s="87" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" s="95" t="s">
         <v>245</v>
       </c>
-      <c r="B29" s="104" t="s">
+      <c r="C29" s="96">
+        <v>-209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="C29" s="105">
-        <v>-209</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="123" t="s">
+      <c r="B30" s="107" t="s">
         <v>247</v>
       </c>
-      <c r="B30" s="116" t="s">
+      <c r="C30" s="94">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="87" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="103">
+      <c r="B31" s="95" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" s="96">
+        <v>-628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="114" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="107" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" s="94">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="96" t="s">
-        <v>249</v>
-      </c>
-      <c r="B31" s="104" t="s">
-        <v>246</v>
-      </c>
-      <c r="C31" s="105">
-        <v>-628</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="123" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="114" t="s">
         <v>250</v>
       </c>
-      <c r="B32" s="116" t="s">
-        <v>248</v>
-      </c>
-      <c r="C32" s="103">
+      <c r="B33" s="107" t="s">
+        <v>247</v>
+      </c>
+      <c r="C33" s="94">
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="123" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="114" t="s">
+        <v>250</v>
+      </c>
+      <c r="B34" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="B33" s="116" t="s">
-        <v>248</v>
-      </c>
-      <c r="C33" s="103">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="123" t="s">
-        <v>251</v>
-      </c>
-      <c r="B34" s="116" t="s">
+      <c r="C34" s="94">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="114" t="s">
         <v>252</v>
       </c>
-      <c r="C34" s="103">
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="123" t="s">
+      <c r="B35" s="107" t="s">
         <v>253</v>
       </c>
-      <c r="B35" s="116" t="s">
+      <c r="C35" s="94">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="115">
+        <v>42906</v>
+      </c>
+      <c r="B36" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="C35" s="103">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="124">
-        <v>42906</v>
-      </c>
-      <c r="B36" s="125" t="s">
-        <v>255</v>
-      </c>
-      <c r="C36" s="126">
+      <c r="C36" s="117">
         <v>-188</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="106"/>
-      <c r="B37" s="107" t="s">
+      <c r="A37" s="97"/>
+      <c r="B37" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="108">
+      <c r="C37" s="99">
         <f>SUM(C29:C36)</f>
         <v>-256</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="127" t="s">
+      <c r="A40" s="150" t="s">
+        <v>255</v>
+      </c>
+      <c r="B40" s="151"/>
+      <c r="C40" s="152"/>
+    </row>
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="109" t="s">
         <v>256</v>
       </c>
-      <c r="B40" s="128"/>
-      <c r="C40" s="129"/>
-    </row>
-    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="118" t="s">
+      <c r="B41" s="110">
+        <v>604</v>
+      </c>
+      <c r="C41" s="86"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="91" t="s">
         <v>257</v>
       </c>
-      <c r="B41" s="119">
-        <v>604</v>
-      </c>
-      <c r="C41" s="95"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="100" t="s">
+      <c r="B42" s="21"/>
+      <c r="C42" s="86"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="118" t="s">
         <v>258</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="95"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="130" t="s">
-        <v>259</v>
-      </c>
-      <c r="B43" s="131">
+      <c r="B43" s="119">
         <f>C46</f>
         <v>-604</v>
       </c>
-      <c r="C43" s="95"/>
+      <c r="C43" s="86"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="100" t="s">
-        <v>224</v>
-      </c>
-      <c r="C44" s="95"/>
+      <c r="A44" s="91" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" s="86"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="100"/>
-      <c r="C45" s="95"/>
+      <c r="A45" s="91"/>
+      <c r="C45" s="86"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="96" t="s">
+      <c r="A46" s="87" t="s">
+        <v>259</v>
+      </c>
+      <c r="B46" s="120" t="s">
         <v>260</v>
       </c>
-      <c r="B46" s="132" t="s">
+      <c r="C46" s="121">
+        <v>-604</v>
+      </c>
+      <c r="D46" s="139"/>
+      <c r="E46" s="139"/>
+      <c r="F46" s="139"/>
+      <c r="G46" s="139"/>
+      <c r="H46" s="139"/>
+      <c r="I46" s="139"/>
+      <c r="J46" s="139"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="114" t="s">
         <v>261</v>
       </c>
-      <c r="C46" s="133">
-        <v>-604</v>
-      </c>
-      <c r="D46" s="88"/>
-      <c r="E46" s="88"/>
-      <c r="F46" s="88"/>
-      <c r="G46" s="88"/>
-      <c r="H46" s="88"/>
-      <c r="I46" s="88"/>
-      <c r="J46" s="88"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="123" t="s">
+      <c r="B47" s="107" t="s">
+        <v>253</v>
+      </c>
+      <c r="C47" s="122">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="B47" s="116" t="s">
-        <v>254</v>
-      </c>
-      <c r="C47" s="134">
+      <c r="B48" s="107" t="s">
+        <v>253</v>
+      </c>
+      <c r="C48" s="122">
         <v>192</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="123" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="B49" s="107" t="s">
         <v>263</v>
       </c>
-      <c r="B48" s="116" t="s">
-        <v>254</v>
-      </c>
-      <c r="C48" s="134">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="135" t="s">
-        <v>263</v>
-      </c>
-      <c r="B49" s="116" t="s">
+      <c r="C49" s="94">
+        <v>-82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="123" t="s">
         <v>264</v>
       </c>
-      <c r="C49" s="103">
-        <v>-82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="135" t="s">
+      <c r="B50" s="107" t="s">
         <v>265</v>
       </c>
-      <c r="B50" s="116" t="s">
+      <c r="C50" s="122">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="123" t="s">
         <v>266</v>
       </c>
-      <c r="C50" s="134">
+      <c r="B51" s="107" t="s">
+        <v>265</v>
+      </c>
+      <c r="C51" s="122">
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="135" t="s">
-        <v>267</v>
-      </c>
-      <c r="B51" s="116" t="s">
-        <v>266</v>
-      </c>
-      <c r="C51" s="134">
-        <v>151</v>
-      </c>
-    </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="106"/>
-      <c r="B52" s="107" t="s">
+      <c r="A52" s="97"/>
+      <c r="B52" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="108">
+      <c r="C52" s="99">
         <f>SUM(C46:C51)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="136" t="s">
+      <c r="A55" s="141" t="s">
+        <v>267</v>
+      </c>
+      <c r="B55" s="142"/>
+      <c r="C55" s="143"/>
+    </row>
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="124" t="s">
         <v>268</v>
       </c>
-      <c r="B55" s="137"/>
-      <c r="C55" s="138"/>
-    </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="139" t="s">
+      <c r="B56" s="21"/>
+      <c r="C56" s="125"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="126" t="s">
         <v>269</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="140"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="141" t="s">
+      <c r="B57" s="21"/>
+      <c r="C57" s="125"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="126" t="s">
         <v>270</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="140"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="141" t="s">
+      <c r="B58" s="21"/>
+      <c r="C58" s="125"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="126" t="s">
+        <v>223</v>
+      </c>
+      <c r="C59" s="125"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="126"/>
+      <c r="C60" s="125"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="127" t="s">
         <v>271</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="140"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="141" t="s">
-        <v>224</v>
-      </c>
-      <c r="C59" s="140"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="141"/>
-      <c r="C60" s="140"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="142" t="s">
+      <c r="B61" s="107" t="s">
         <v>272</v>
       </c>
-      <c r="B61" s="116" t="s">
+      <c r="C61" s="128">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="129">
+        <v>43592</v>
+      </c>
+      <c r="B62" s="107" t="s">
         <v>273</v>
       </c>
-      <c r="C61" s="143">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="144">
-        <v>43592</v>
-      </c>
-      <c r="B62" s="116" t="s">
+      <c r="C62" s="128">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="130">
+        <v>43594</v>
+      </c>
+      <c r="B63" s="95" t="s">
         <v>274</v>
       </c>
-      <c r="C62" s="143">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="145">
-        <v>43594</v>
-      </c>
-      <c r="B63" s="104" t="s">
-        <v>275</v>
-      </c>
-      <c r="C63" s="105">
+      <c r="C63" s="96">
         <f>-B74</f>
         <v>-1482</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="142" t="s">
-        <v>276</v>
-      </c>
-      <c r="B64" s="116" t="s">
-        <v>273</v>
-      </c>
-      <c r="C64" s="143">
+      <c r="A64" s="127" t="s">
+        <v>275</v>
+      </c>
+      <c r="B64" s="107" t="s">
+        <v>272</v>
+      </c>
+      <c r="C64" s="128">
         <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="59" t="s">
-        <v>277</v>
-      </c>
-      <c r="B67" s="146">
+        <v>276</v>
+      </c>
+      <c r="B67" s="131">
         <f>C8+C20+C37+C52+SUM(C61:C64)</f>
         <v>-941</v>
       </c>
       <c r="D67" s="82" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D68" s="82" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="82" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D69" s="82" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="82" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B70" s="15">
         <v>592</v>
       </c>
       <c r="D70" s="82" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="82" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B71" s="15">
         <v>1243</v>
       </c>
       <c r="D71" s="82" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="82" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B72" s="15">
         <v>151</v>
@@ -4266,7 +4280,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="82" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B73" s="15">
         <v>202</v>
@@ -4280,71 +4294,92 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="82" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="144" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="147" t="s">
-        <v>284</v>
-      </c>
-      <c r="B76" s="147"/>
+      <c r="B76" s="144"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="147"/>
-      <c r="B77" s="147"/>
+      <c r="A77" s="144"/>
+      <c r="B77" s="144"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="82" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="82" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="145" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="148" t="s">
-        <v>287</v>
-      </c>
-      <c r="B80" s="148"/>
+      <c r="B80" s="145"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="149"/>
-      <c r="B81" s="149"/>
+      <c r="A81" s="146"/>
+      <c r="B81" s="146"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="82" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="82" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="150" t="s">
-        <v>291</v>
+      <c r="A85" s="132" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="82" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="82" t="s">
-        <v>293</v>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A88" s="59" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="82" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="83" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="133" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
     <mergeCell ref="A80:B81"/>
@@ -4352,7 +4387,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5016,20 +5050,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="135" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="8" t="s">
@@ -5167,11 +5201,11 @@
       <c r="B15" s="43">
         <v>438.04</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="136" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
@@ -5196,20 +5230,20 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="137" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="46" t="s">
@@ -5303,10 +5337,10 @@
         <f>ROUND((B33-18000)*0.35+1750,2)</f>
         <v>5779.41</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="138" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="88"/>
+      <c r="D34" s="139"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="41" t="s">
@@ -5316,10 +5350,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>244.34</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="139" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="88"/>
+      <c r="D35" s="139"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="44" t="s">
@@ -5394,10 +5428,10 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="83" t="s">
+      <c r="A53" s="134" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="83"/>
+      <c r="B53" s="134"/>
     </row>
     <row r="54" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="61" t="s">
@@ -6686,32 +6720,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="135" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="G1" s="84" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="G1" s="135" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="8" t="s">
@@ -6954,22 +6988,22 @@
       <c r="B15" s="43">
         <v>1535.69</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="136" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
       <c r="G15" s="42" t="s">
         <v>132</v>
       </c>
       <c r="H15" s="43">
         <v>413.13</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="136" t="s">
         <v>133</v>
       </c>
-      <c r="J15" s="85"/>
-      <c r="K15" s="85"/>
+      <c r="J15" s="136"/>
+      <c r="K15" s="136"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
@@ -7010,20 +7044,20 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="137" t="s">
         <v>158</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="46" t="s">
@@ -7120,10 +7154,10 @@
         <f>ROUND((B33-31000)*0.42+6300,2)</f>
         <v>7195.15</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="88"/>
+      <c r="D34" s="139"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="41" t="s">
@@ -7133,10 +7167,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>312.08999999999997</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="139" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="88"/>
+      <c r="D35" s="139"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="44" t="s">
@@ -7212,10 +7246,10 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="83" t="s">
+      <c r="A53" s="134" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="83"/>
+      <c r="B53" s="134"/>
     </row>
     <row r="54" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="61" t="s">
@@ -8495,7 +8529,7 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8520,44 +8554,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="135" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="G1" s="84" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="G1" s="135" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="M1" s="84" t="s">
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="M1" s="135" t="s">
         <v>180</v>
       </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="135"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C3" s="71" t="s">
@@ -8905,25 +8939,25 @@
       <c r="B15" s="43">
         <v>175.89</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="136" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
       <c r="G15" s="42" t="s">
         <v>132</v>
       </c>
       <c r="H15" s="43">
         <v>13.93</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="136" t="s">
         <v>133</v>
       </c>
-      <c r="J15" s="85"/>
-      <c r="K15" s="85"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
+      <c r="J15" s="136"/>
+      <c r="K15" s="136"/>
+      <c r="O15" s="140"/>
+      <c r="P15" s="140"/>
+      <c r="Q15" s="140"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
@@ -8974,20 +9008,20 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="137" t="s">
         <v>177</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="46" t="s">
@@ -9074,10 +9108,10 @@
         <f>ROUND((B32-31000)*0.42+6300,2)</f>
         <v>8538.18</v>
       </c>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="88"/>
+      <c r="D33" s="139"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="41" t="s">
@@ -9087,10 +9121,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>329.36</v>
       </c>
-      <c r="C34" s="88" t="s">
+      <c r="C34" s="139" t="s">
         <v>147</v>
       </c>
-      <c r="D34" s="88"/>
+      <c r="D34" s="139"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="44" t="s">
@@ -9165,10 +9199,10 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="83" t="s">
+      <c r="A51" s="134" t="s">
         <v>183</v>
       </c>
-      <c r="B51" s="83"/>
+      <c r="B51" s="134"/>
     </row>
     <row r="52" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="61" t="s">
@@ -10299,8 +10333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDD0FDF-F307-4A0B-AA7E-FBECBEA542D5}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A25" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10325,44 +10359,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="135" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="G1" s="84" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="G1" s="135" t="s">
         <v>189</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="M1" s="84" t="s">
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="M1" s="135" t="s">
         <v>202</v>
       </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="135"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C3" s="73" t="s">
@@ -10721,12 +10755,12 @@
       <c r="H15" s="43">
         <v>12.87</v>
       </c>
-      <c r="I15" s="85"/>
-      <c r="J15" s="85"/>
-      <c r="K15" s="85"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
+      <c r="I15" s="136"/>
+      <c r="J15" s="136"/>
+      <c r="K15" s="136"/>
+      <c r="O15" s="140"/>
+      <c r="P15" s="140"/>
+      <c r="Q15" s="140"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
@@ -10776,20 +10810,20 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="137" t="s">
         <v>191</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="46" t="s">
@@ -10876,10 +10910,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>9144.59</v>
       </c>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="88"/>
+      <c r="D33" s="139"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="41" t="s">
@@ -10889,10 +10923,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>331.57</v>
       </c>
-      <c r="C34" s="88" t="s">
+      <c r="C34" s="139" t="s">
         <v>147</v>
       </c>
-      <c r="D34" s="88"/>
+      <c r="D34" s="139"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="44" t="s">
@@ -10963,14 +10997,14 @@
         <v>1761.0000000000005</v>
       </c>
       <c r="C44" s="74" t="s">
-        <v>216</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="83" t="s">
+      <c r="A51" s="134" t="s">
         <v>214</v>
       </c>
-      <c r="B51" s="83"/>
+      <c r="B51" s="134"/>
     </row>
     <row r="52" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="61" t="s">

</xml_diff>

<commit_message>
Steuervorauszahlung 3 und 4. Quartal 2022
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1501FE92-879B-0243-BBDB-1C9E4CD301FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911192E9-EA5C-5147-B72D-7DEE0C08E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="26580" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26580" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="352">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1113,6 +1113,18 @@
   </si>
   <si>
     <t>Stand 21.04.2022</t>
+  </si>
+  <si>
+    <t>Stand 22.07.2022</t>
+  </si>
+  <si>
+    <t>Neuen Quartalsberechnungen für 2022 erhalten und ergeben 1.Q: 781€;  2.Q: 781€;  3.Q: 880€;  4.Q: 815€ (Summe 3257€)</t>
+  </si>
+  <si>
+    <t>Ergibt folgende Überweisung 1.Q und 2.Q wurde schon überwiesen;  3.Q + 4.Q = 880 +815 = 1695€</t>
+  </si>
+  <si>
+    <t>Am 22.4.2022 wurden 1695€ überwiesen und dies sollte bis Jahresende reichen, d.h. am 1.1.2023 sollte Kontostand auf 0 sein.</t>
   </si>
 </sst>
 </file>
@@ -2801,6 +2813,11 @@
     <xf numFmtId="49" fontId="24" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2820,9 +2837,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2852,8 +2866,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7716,7 +7728,7 @@
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
@@ -10731,10 +10743,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A86" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10747,11 +10759,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="280" t="s">
+      <c r="A1" s="282" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="282"/>
+      <c r="B1" s="283"/>
+      <c r="C1" s="284"/>
       <c r="D1" s="164"/>
       <c r="E1" s="41" t="s">
         <v>233</v>
@@ -10919,11 +10931,11 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="283" t="s">
+      <c r="A11" s="285" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="284"/>
-      <c r="C11" s="282"/>
+      <c r="B11" s="286"/>
+      <c r="C11" s="284"/>
       <c r="D11" s="164"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -11107,11 +11119,11 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="283" t="s">
+      <c r="A23" s="285" t="s">
         <v>260</v>
       </c>
-      <c r="B23" s="284"/>
-      <c r="C23" s="282"/>
+      <c r="B23" s="286"/>
+      <c r="C23" s="284"/>
       <c r="D23" s="164"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -11387,11 +11399,11 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="285" t="s">
+      <c r="A40" s="287" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="286"/>
-      <c r="C40" s="287"/>
+      <c r="B40" s="288"/>
+      <c r="C40" s="289"/>
       <c r="D40" s="164"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -11483,7 +11495,7 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="271"/>
+      <c r="D46" s="274"/>
       <c r="E46" s="254"/>
       <c r="F46" s="254"/>
       <c r="G46" s="254"/>
@@ -11623,11 +11635,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="272" t="s">
+      <c r="A55" s="275" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="273"/>
-      <c r="C55" s="274"/>
+      <c r="B55" s="276"/>
+      <c r="C55" s="277"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -11938,10 +11950,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="275" t="s">
+      <c r="A76" s="278" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="276"/>
+      <c r="B76" s="279"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -11952,8 +11964,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="277"/>
-      <c r="B77" s="276"/>
+      <c r="A77" s="280"/>
+      <c r="B77" s="279"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -11992,10 +12004,10 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="278" t="s">
+      <c r="A80" s="271" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="279"/>
+      <c r="B80" s="281"/>
       <c r="C80" s="64"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -12006,8 +12018,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="277"/>
-      <c r="B81" s="276"/>
+      <c r="A81" s="280"/>
+      <c r="B81" s="279"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -12214,10 +12226,10 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="278" t="s">
+      <c r="A96" s="271" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="288"/>
+      <c r="B96" s="272"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -12228,7 +12240,7 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="289"/>
+      <c r="A97" s="273"/>
       <c r="B97" s="265"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
@@ -12337,9 +12349,11 @@
       <c r="I104" s="11"/>
       <c r="J104" s="11"/>
     </row>
-    <row r="105" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="11"/>
-      <c r="B105" s="11"/>
+    <row r="105" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="230" t="s">
+        <v>348</v>
+      </c>
+      <c r="B105" s="76"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
@@ -12350,7 +12364,9 @@
       <c r="J105" s="11"/>
     </row>
     <row r="106" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="11"/>
+      <c r="A106" s="236" t="s">
+        <v>349</v>
+      </c>
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -12361,17 +12377,29 @@
       <c r="I106" s="11"/>
       <c r="J106" s="11"/>
     </row>
+    <row r="107" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B107" s="11"/>
+    </row>
+    <row r="108" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="235" t="s">
+        <v>351</v>
+      </c>
+      <c r="B108" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A96:B97"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
     <mergeCell ref="A80:B81"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Steuer Update (Einzahlung 1.Q 2023)
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8266256F-0A54-E44E-9924-28E0F8CAD02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7282B5-6B53-0643-BAC3-07D0D8A01DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26580" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="356">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1126,6 +1126,18 @@
   <si>
     <t>Am 25.7.2022 wurden 1695€ überwiesen und dies sollte bis Jahresende reichen, d.h. am 1.1.2023 sollte Kontostand auf 0 sein.</t>
   </si>
+  <si>
+    <t>Korrekt mit 1.1.2023 ist der Kontostand auf 0€!</t>
+  </si>
+  <si>
+    <t>Stand 10.02.2023</t>
+  </si>
+  <si>
+    <t>Bescheid bekommen über die Vorauszahlung für 2023. Diese ergibt 3257€ (1.Q: 814€;  2.Q: 814€;  3.Q: 814€;  4.Q: 815€), selber Betrag wie 2022, d.h dieser Betrag wird sich noch ändern sobald die Steuererklärung für 2022 gemacht wurde.</t>
+  </si>
+  <si>
+    <t>Am 10.02.2023 wurden 814€ überwiesen wegen 1.Q. Der Betrag für das 2.Q ist erst am 15.05 Fällig. Bis dahin habe ich eventuell schon die aktualisierte Vorausberechnung für 2023 und dann könnte man die restliche Jahressumme überweisen.</t>
+  </si>
 </sst>
 </file>
 
@@ -1142,7 +1154,7 @@
     <numFmt numFmtId="171" formatCode="[$€-2]&quot; &quot;#,##0.00"/>
     <numFmt numFmtId="172" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="15"/>
       <color indexed="8"/>
@@ -1330,6 +1342,26 @@
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -2439,7 +2471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="290">
+  <cellXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2732,9 +2764,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2743,16 +2772,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2774,8 +2803,8 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2797,7 +2826,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="24" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2811,6 +2840,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="24" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2837,35 +2893,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="35" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4053,11 +4088,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="242" t="s">
+      <c r="B3" s="241" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="243"/>
-      <c r="D3" s="243"/>
+      <c r="C3" s="242"/>
+      <c r="D3" s="242"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4299,46 +4334,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="266"/>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
+      <c r="A1" s="265"/>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="267" t="s">
+      <c r="G1" s="266" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="259"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="258"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="267" t="s">
+      <c r="M1" s="266" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="259"/>
-      <c r="O1" s="259"/>
-      <c r="P1" s="259"/>
-      <c r="Q1" s="260"/>
+      <c r="N1" s="258"/>
+      <c r="O1" s="258"/>
+      <c r="P1" s="258"/>
+      <c r="Q1" s="259"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="255"/>
-      <c r="B2" s="261"/>
-      <c r="C2" s="261"/>
-      <c r="D2" s="261"/>
-      <c r="E2" s="261"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="260"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="261"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="261"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="260"/>
+      <c r="I2" s="260"/>
+      <c r="J2" s="260"/>
+      <c r="K2" s="260"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="261"/>
-      <c r="N2" s="261"/>
-      <c r="O2" s="261"/>
-      <c r="P2" s="261"/>
-      <c r="Q2" s="262"/>
+      <c r="M2" s="260"/>
+      <c r="N2" s="260"/>
+      <c r="O2" s="260"/>
+      <c r="P2" s="260"/>
+      <c r="Q2" s="261"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -4788,15 +4823,15 @@
       <c r="H15" s="63">
         <v>12.87</v>
       </c>
-      <c r="I15" s="268"/>
-      <c r="J15" s="252"/>
-      <c r="K15" s="252"/>
+      <c r="I15" s="267"/>
+      <c r="J15" s="251"/>
+      <c r="K15" s="251"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="265"/>
-      <c r="P15" s="265"/>
-      <c r="Q15" s="265"/>
+      <c r="O15" s="264"/>
+      <c r="P15" s="264"/>
+      <c r="Q15" s="264"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
@@ -4918,13 +4953,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="269" t="s">
+      <c r="A21" s="268" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="264"/>
-      <c r="C21" s="264"/>
-      <c r="D21" s="264"/>
-      <c r="E21" s="264"/>
+      <c r="B21" s="263"/>
+      <c r="C21" s="263"/>
+      <c r="D21" s="263"/>
+      <c r="E21" s="263"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -4939,11 +4974,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="264"/>
-      <c r="B22" s="264"/>
-      <c r="C22" s="264"/>
-      <c r="D22" s="264"/>
-      <c r="E22" s="264"/>
+      <c r="A22" s="263"/>
+      <c r="B22" s="263"/>
+      <c r="C22" s="263"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="263"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -5192,10 +5227,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>9144.59</v>
       </c>
-      <c r="C33" s="253" t="s">
+      <c r="C33" s="252" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="254"/>
+      <c r="D33" s="253"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -5218,10 +5253,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>331.57</v>
       </c>
-      <c r="C34" s="253" t="s">
+      <c r="C34" s="252" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="254"/>
+      <c r="D34" s="253"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -5518,10 +5553,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="249" t="s">
+      <c r="A48" s="248" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="250"/>
+      <c r="B48" s="249"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -7753,34 +7788,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="267" t="s">
+      <c r="A1" s="266" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="267"/>
-      <c r="C1" s="267"/>
-      <c r="D1" s="267"/>
-      <c r="E1" s="267"/>
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="266"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="267" t="s">
+      <c r="G1" s="266" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="260"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="259"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="270"/>
-      <c r="B2" s="270"/>
-      <c r="C2" s="270"/>
-      <c r="D2" s="270"/>
-      <c r="E2" s="270"/>
+      <c r="A2" s="269"/>
+      <c r="B2" s="269"/>
+      <c r="C2" s="269"/>
+      <c r="D2" s="269"/>
+      <c r="E2" s="269"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="261"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="262"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="260"/>
+      <c r="I2" s="260"/>
+      <c r="J2" s="260"/>
+      <c r="K2" s="261"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -7875,13 +7910,13 @@
     <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="50"/>
       <c r="B7" s="51"/>
-      <c r="C7" s="238"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="53"/>
       <c r="E7" s="53"/>
       <c r="F7" s="11"/>
       <c r="G7" s="50"/>
       <c r="H7" s="51"/>
-      <c r="I7" s="238"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="53"/>
       <c r="K7" s="53"/>
     </row>
@@ -7991,13 +8026,13 @@
     <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60"/>
       <c r="B11" s="42"/>
-      <c r="C11" s="238"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="61"/>
       <c r="E11" s="61"/>
       <c r="F11" s="11"/>
       <c r="G11" s="60"/>
       <c r="H11" s="42"/>
-      <c r="I11" s="238"/>
+      <c r="I11" s="52"/>
       <c r="J11" s="61"/>
       <c r="K11" s="61"/>
     </row>
@@ -8079,15 +8114,15 @@
       <c r="B15" s="63">
         <v>3.91</v>
       </c>
-      <c r="C15" s="239"/>
+      <c r="C15" s="238"/>
       <c r="D15" s="237"/>
       <c r="E15" s="237"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="265"/>
-      <c r="J15" s="265"/>
-      <c r="K15" s="265"/>
+      <c r="I15" s="264"/>
+      <c r="J15" s="264"/>
+      <c r="K15" s="264"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="127" t="s">
@@ -8191,13 +8226,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="269" t="s">
+      <c r="A21" s="268" t="s">
         <v>330</v>
       </c>
-      <c r="B21" s="264"/>
-      <c r="C21" s="264"/>
-      <c r="D21" s="264"/>
-      <c r="E21" s="264"/>
+      <c r="B21" s="263"/>
+      <c r="C21" s="263"/>
+      <c r="D21" s="263"/>
+      <c r="E21" s="263"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -8212,11 +8247,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="264"/>
-      <c r="B22" s="264"/>
-      <c r="C22" s="264"/>
-      <c r="D22" s="264"/>
-      <c r="E22" s="264"/>
+      <c r="A22" s="263"/>
+      <c r="B22" s="263"/>
+      <c r="C22" s="263"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="263"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -8465,10 +8500,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>10076.74</v>
       </c>
-      <c r="C33" s="253" t="s">
+      <c r="C33" s="252" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="254"/>
+      <c r="D33" s="253"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -8491,10 +8526,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>337.3</v>
       </c>
-      <c r="C34" s="253" t="s">
+      <c r="C34" s="252" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="254"/>
+      <c r="D34" s="253"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -8791,10 +8826,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="249" t="s">
+      <c r="A48" s="248" t="s">
         <v>331</v>
       </c>
-      <c r="B48" s="250"/>
+      <c r="B48" s="249"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -8975,7 +9010,7 @@
   </sheetPr>
   <dimension ref="A1:AZ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -9215,7 +9250,7 @@
         <f>B9+B11</f>
         <v>228.5800000000001</v>
       </c>
-      <c r="H8" s="241">
+      <c r="H8" s="240">
         <f>B12</f>
         <v>275.76</v>
       </c>
@@ -10600,52 +10635,52 @@
       <c r="AJ44" s="103">
         <v>2.4</v>
       </c>
-      <c r="AK44" s="240">
+      <c r="AK44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AL44" s="240">
+      <c r="AL44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AM44" s="240">
+      <c r="AM44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AN44" s="240">
+      <c r="AN44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AO44" s="240">
+      <c r="AO44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AP44" s="240">
+      <c r="AP44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AQ44" s="240">
+      <c r="AQ44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AR44" s="240">
+      <c r="AR44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AS44" s="240">
+      <c r="AS44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AT44" s="240">
+      <c r="AT44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AU44" s="240">
+      <c r="AU44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AV44" s="240">
+      <c r="AV44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AW44" s="240">
+      <c r="AW44" s="239">
         <v>2.9</v>
       </c>
-      <c r="AX44" s="240">
+      <c r="AX44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AY44" s="240">
+      <c r="AY44" s="239">
         <v>4.2</v>
       </c>
-      <c r="AZ44" s="240">
+      <c r="AZ44" s="239">
         <v>2.9</v>
       </c>
     </row>
@@ -10743,10 +10778,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A93" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10759,11 +10794,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="279" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="272"/>
-      <c r="C1" s="273"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="281"/>
       <c r="D1" s="164"/>
       <c r="E1" s="41" t="s">
         <v>233</v>
@@ -10907,7 +10942,7 @@
       <c r="B9" s="187"/>
       <c r="C9" s="187"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="292" t="s">
         <v>247</v>
       </c>
       <c r="F9" s="11"/>
@@ -10931,11 +10966,11 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="274" t="s">
+      <c r="A11" s="282" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="275"/>
-      <c r="C11" s="273"/>
+      <c r="B11" s="283"/>
+      <c r="C11" s="281"/>
       <c r="D11" s="164"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -11119,11 +11154,11 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="274" t="s">
+      <c r="A23" s="282" t="s">
         <v>260</v>
       </c>
-      <c r="B23" s="275"/>
-      <c r="C23" s="273"/>
+      <c r="B23" s="283"/>
+      <c r="C23" s="281"/>
       <c r="D23" s="164"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -11399,11 +11434,11 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="276" t="s">
+      <c r="A40" s="284" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="277"/>
-      <c r="C40" s="278"/>
+      <c r="B40" s="285"/>
+      <c r="C40" s="286"/>
       <c r="D40" s="164"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -11495,13 +11530,13 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="282"/>
-      <c r="E46" s="254"/>
-      <c r="F46" s="254"/>
-      <c r="G46" s="254"/>
-      <c r="H46" s="254"/>
-      <c r="I46" s="254"/>
-      <c r="J46" s="254"/>
+      <c r="D46" s="270"/>
+      <c r="E46" s="253"/>
+      <c r="F46" s="253"/>
+      <c r="G46" s="253"/>
+      <c r="H46" s="253"/>
+      <c r="I46" s="253"/>
+      <c r="J46" s="253"/>
     </row>
     <row r="47" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="180" t="s">
@@ -11635,11 +11670,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="283" t="s">
+      <c r="A55" s="271" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="284"/>
-      <c r="C55" s="285"/>
+      <c r="B55" s="272"/>
+      <c r="C55" s="273"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -11950,10 +11985,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="286" t="s">
+      <c r="A76" s="274" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="287"/>
+      <c r="B76" s="275"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -11964,8 +11999,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="288"/>
-      <c r="B77" s="287"/>
+      <c r="A77" s="276"/>
+      <c r="B77" s="275"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -12004,10 +12039,10 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="279" t="s">
+      <c r="A80" s="277" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="289"/>
+      <c r="B80" s="278"/>
       <c r="C80" s="64"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -12018,8 +12053,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="288"/>
-      <c r="B81" s="287"/>
+      <c r="A81" s="276"/>
+      <c r="B81" s="275"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -12226,10 +12261,10 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="279" t="s">
+      <c r="A96" s="277" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="280"/>
+      <c r="B96" s="287"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -12240,8 +12275,8 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="281"/>
-      <c r="B97" s="265"/>
+      <c r="A97" s="288"/>
+      <c r="B97" s="264"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -12389,8 +12424,38 @@
       </c>
       <c r="B108" s="11"/>
     </row>
+    <row r="109" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="289" t="s">
+        <v>352</v>
+      </c>
+      <c r="B109" s="287"/>
+    </row>
+    <row r="110" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="288"/>
+      <c r="B110" s="264"/>
+    </row>
+    <row r="111" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="290" t="s">
+        <v>353</v>
+      </c>
+      <c r="B111" s="76"/>
+    </row>
+    <row r="112" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="291" t="s">
+        <v>354</v>
+      </c>
+      <c r="B112" s="11"/>
+    </row>
+    <row r="113" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="292" t="s">
+        <v>355</v>
+      </c>
+      <c r="B113" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A96:B97"/>
+    <mergeCell ref="A109:B110"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
@@ -12399,7 +12464,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A96:B97"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
@@ -14580,20 +14644,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="244" t="s">
+      <c r="A1" s="243" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="246"/>
+      <c r="B1" s="244"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="245"/>
     </row>
     <row r="2" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="255"/>
-      <c r="B2" s="256"/>
-      <c r="C2" s="256"/>
-      <c r="D2" s="256"/>
-      <c r="E2" s="257"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="255"/>
+      <c r="C2" s="255"/>
+      <c r="D2" s="255"/>
+      <c r="E2" s="256"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -14753,11 +14817,11 @@
       <c r="B15" s="63">
         <v>438.04</v>
       </c>
-      <c r="C15" s="251" t="s">
+      <c r="C15" s="250" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="252"/>
-      <c r="E15" s="252"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
     </row>
     <row r="16" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -14805,20 +14869,20 @@
       <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="247" t="s">
+      <c r="A21" s="246" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
+      <c r="B21" s="247"/>
+      <c r="C21" s="247"/>
+      <c r="D21" s="247"/>
+      <c r="E21" s="247"/>
     </row>
     <row r="22" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="248"/>
-      <c r="B22" s="248"/>
-      <c r="C22" s="248"/>
-      <c r="D22" s="248"/>
-      <c r="E22" s="248"/>
+      <c r="A22" s="247"/>
+      <c r="B22" s="247"/>
+      <c r="C22" s="247"/>
+      <c r="D22" s="247"/>
+      <c r="E22" s="247"/>
     </row>
     <row r="23" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
@@ -14946,10 +15010,10 @@
         <f>ROUND((B33-18000)*0.35+1750,2)</f>
         <v>5779.41</v>
       </c>
-      <c r="C34" s="253" t="s">
+      <c r="C34" s="252" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="254"/>
+      <c r="D34" s="253"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14960,10 +15024,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>244.34</v>
       </c>
-      <c r="C35" s="253" t="s">
+      <c r="C35" s="252" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="254"/>
+      <c r="D35" s="253"/>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15090,10 +15154,10 @@
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="249" t="s">
+      <c r="A49" s="248" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="250"/>
+      <c r="B49" s="249"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -18474,34 +18538,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="262" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="258" t="s">
+      <c r="G1" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="260"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="259"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="255"/>
-      <c r="B2" s="261"/>
-      <c r="C2" s="261"/>
-      <c r="D2" s="261"/>
-      <c r="E2" s="261"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="260"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="261"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="262"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="260"/>
+      <c r="I2" s="260"/>
+      <c r="J2" s="260"/>
+      <c r="K2" s="261"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -18800,11 +18864,11 @@
       <c r="B15" s="63">
         <v>1535.69</v>
       </c>
-      <c r="C15" s="251" t="s">
+      <c r="C15" s="250" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="252"/>
-      <c r="E15" s="252"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -18812,11 +18876,11 @@
       <c r="H15" s="63">
         <v>413.13</v>
       </c>
-      <c r="I15" s="251" t="s">
+      <c r="I15" s="250" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="252"/>
-      <c r="K15" s="252"/>
+      <c r="J15" s="251"/>
+      <c r="K15" s="251"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -18904,13 +18968,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="247" t="s">
+      <c r="A21" s="246" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="264"/>
-      <c r="C21" s="264"/>
-      <c r="D21" s="264"/>
-      <c r="E21" s="264"/>
+      <c r="B21" s="263"/>
+      <c r="C21" s="263"/>
+      <c r="D21" s="263"/>
+      <c r="E21" s="263"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -18919,11 +18983,11 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="264"/>
-      <c r="B22" s="264"/>
-      <c r="C22" s="264"/>
-      <c r="D22" s="264"/>
-      <c r="E22" s="264"/>
+      <c r="A22" s="263"/>
+      <c r="B22" s="263"/>
+      <c r="C22" s="263"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="263"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -19124,10 +19188,10 @@
         <f>ROUND((B33-31000)*0.42+6300,2)</f>
         <v>7196.73</v>
       </c>
-      <c r="C34" s="253" t="s">
+      <c r="C34" s="252" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="254"/>
+      <c r="D34" s="253"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -19144,10 +19208,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>312.08999999999997</v>
       </c>
-      <c r="C35" s="253" t="s">
+      <c r="C35" s="252" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="254"/>
+      <c r="D35" s="253"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -19371,10 +19435,10 @@
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="249" t="s">
+      <c r="A50" s="248" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="250"/>
+      <c r="B50" s="249"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -23146,48 +23210,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="262" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="258" t="s">
+      <c r="G1" s="257" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="259"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="258"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="258" t="s">
+      <c r="M1" s="257" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="259"/>
-      <c r="O1" s="259"/>
-      <c r="P1" s="259"/>
-      <c r="Q1" s="260"/>
+      <c r="N1" s="258"/>
+      <c r="O1" s="258"/>
+      <c r="P1" s="258"/>
+      <c r="Q1" s="259"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="255"/>
-      <c r="B2" s="261"/>
-      <c r="C2" s="261"/>
-      <c r="D2" s="261"/>
-      <c r="E2" s="261"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="260"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="261"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="261"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="260"/>
+      <c r="I2" s="260"/>
+      <c r="J2" s="260"/>
+      <c r="K2" s="260"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="261"/>
-      <c r="N2" s="261"/>
-      <c r="O2" s="261"/>
-      <c r="P2" s="261"/>
-      <c r="Q2" s="262"/>
+      <c r="M2" s="260"/>
+      <c r="N2" s="260"/>
+      <c r="O2" s="260"/>
+      <c r="P2" s="260"/>
+      <c r="Q2" s="261"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -23625,11 +23689,11 @@
       <c r="B15" s="63">
         <v>175.89</v>
       </c>
-      <c r="C15" s="251" t="s">
+      <c r="C15" s="250" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="252"/>
-      <c r="E15" s="252"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -23637,17 +23701,17 @@
       <c r="H15" s="63">
         <v>13.93</v>
       </c>
-      <c r="I15" s="251" t="s">
+      <c r="I15" s="250" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="252"/>
-      <c r="K15" s="252"/>
+      <c r="J15" s="251"/>
+      <c r="K15" s="251"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="265"/>
-      <c r="P15" s="265"/>
-      <c r="Q15" s="265"/>
+      <c r="O15" s="264"/>
+      <c r="P15" s="264"/>
+      <c r="Q15" s="264"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -23771,13 +23835,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="247" t="s">
+      <c r="A21" s="246" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="264"/>
-      <c r="C21" s="264"/>
-      <c r="D21" s="264"/>
-      <c r="E21" s="264"/>
+      <c r="B21" s="263"/>
+      <c r="C21" s="263"/>
+      <c r="D21" s="263"/>
+      <c r="E21" s="263"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -23792,11 +23856,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="264"/>
-      <c r="B22" s="264"/>
-      <c r="C22" s="264"/>
-      <c r="D22" s="264"/>
-      <c r="E22" s="264"/>
+      <c r="A22" s="263"/>
+      <c r="B22" s="263"/>
+      <c r="C22" s="263"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="263"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -24045,10 +24109,10 @@
         <f>ROUND((B32-31000)*0.42+6300,2)</f>
         <v>8538.18</v>
       </c>
-      <c r="C33" s="253" t="s">
+      <c r="C33" s="252" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="254"/>
+      <c r="D33" s="253"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -24071,10 +24135,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>329.36</v>
       </c>
-      <c r="C34" s="253" t="s">
+      <c r="C34" s="252" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="254"/>
+      <c r="D34" s="253"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -24352,10 +24416,10 @@
       <c r="Q46" s="11"/>
     </row>
     <row r="47" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="249" t="s">
+      <c r="A47" s="248" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="250"/>
+      <c r="B47" s="249"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>

</xml_diff>

<commit_message>
Einkommenssteuererklaerung 2022 first draft
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7282B5-6B53-0643-BAC3-07D0D8A01DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EA755E-D81B-5F46-9D81-D6A90F12BA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26580" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <sheet name="2020" sheetId="11" r:id="rId11"/>
     <sheet name="Berechnung 2021" sheetId="14" r:id="rId12"/>
     <sheet name="2021" sheetId="13" r:id="rId13"/>
-    <sheet name="Steuerkonto" sheetId="12" r:id="rId14"/>
+    <sheet name="Berechnung 2022" sheetId="15" r:id="rId14"/>
+    <sheet name="2022" sheetId="16" r:id="rId15"/>
+    <sheet name="Steuerkonto" sheetId="12" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="382">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -991,6 +993,7 @@
         <sz val="15"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Bis zum nächsten 3.Q (666€ fällig am </t>
     </r>
@@ -1000,6 +1003,7 @@
         <sz val="15"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>16.08.2021</t>
     </r>
@@ -1008,6 +1012,7 @@
         <sz val="15"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>) reicht das, d.h nach dem 17.05.2021 sollte Kontostand auf 0€ sein. (eventuell ergeben sich Änderungen für die Vorauszahlungen 2021, wenn ich bis dahin die Steuererklärung für 2020 gemacht habe)</t>
     </r>
@@ -1137,6 +1142,84 @@
   </si>
   <si>
     <t>Am 10.02.2023 wurden 814€ überwiesen wegen 1.Q. Der Betrag für das 2.Q ist erst am 15.05 Fällig. Bis dahin habe ich eventuell schon die aktualisierte Vorausberechnung für 2023 und dann könnte man die restliche Jahressumme überweisen.</t>
+  </si>
+  <si>
+    <t>Lohnzettel 2022 JKU</t>
+  </si>
+  <si>
+    <t>Berechnungsblatt 2022</t>
+  </si>
+  <si>
+    <t>Vorausbezahlt für das Jahr 2022</t>
+  </si>
+  <si>
+    <t>Zusammenfassung für 2022</t>
+  </si>
+  <si>
+    <t>Sonderzahlung, sprich 13. und 14. Gehalt</t>
+  </si>
+  <si>
+    <t>Lohnzettel 2022 Apple (Part Time 01.01 - 31.03.2022)</t>
+  </si>
+  <si>
+    <t>Lohnzettel 2022 Apple (Full Time 09.05 - 31.12.2022)</t>
+  </si>
+  <si>
+    <t>Steuerfreie Bezüge gemas Paragr. 68</t>
+  </si>
+  <si>
+    <t>ARBEITSMARKTSERVICE ÖSTERREICH (01.04 - 08.05.2022)</t>
+  </si>
+  <si>
+    <t>Tagessatz</t>
+  </si>
+  <si>
+    <t>Anzahl der Tage</t>
+  </si>
+  <si>
+    <t>Gesamtbetrag der Leistungen</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Air Keyboard (mit 40% Privatanteil)</t>
+  </si>
+  <si>
+    <t>Logitech Mouse (mit 40% Privatanteil)</t>
+  </si>
+  <si>
+    <t>Wintersemester 2022/2023</t>
+  </si>
+  <si>
+    <t>Sommersemester 2022</t>
+  </si>
+  <si>
+    <t>mit Grenzsteuersatz von 48%</t>
+  </si>
+  <si>
+    <t>Auguts</t>
+  </si>
+  <si>
+    <t>Septermber</t>
+  </si>
+  <si>
+    <t>Apple Fulltime: Gross Pay (in Euro)</t>
+  </si>
+  <si>
+    <t>RSU (in Dollar)</t>
+  </si>
+  <si>
+    <t>Nebenrechnung um zu checken ob im Jahresbruttogehalt die RSUs enthalten sind</t>
+  </si>
+  <si>
+    <t>Ungenauogkeit wegen Dollar zu Euro Umrechnung, sprich JA ist im Jahresbruttogehalt entahlten</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Anmerkung: Die Gewinne durch ESPP werden nicht beruecksichtigt, also Netto ist noch ein bisschen mehr</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1237,7 @@
     <numFmt numFmtId="171" formatCode="[$€-2]&quot; &quot;#,##0.00"/>
     <numFmt numFmtId="172" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="15"/>
       <color indexed="8"/>
@@ -1164,184 +1247,217 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="17"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="17"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="15"/>
       <color indexed="25"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="15"/>
       <color indexed="27"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="27"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="25"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="29"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="15"/>
       <color indexed="29"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="23"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="17"/>
       <color indexed="25"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="17"/>
       <color indexed="29"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="17"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="17"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="20"/>
       <color indexed="17"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color indexed="27"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="19"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="15"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="25"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="25"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1363,8 +1479,24 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1455,8 +1587,25 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="80">
+  <borders count="81">
     <border>
       <left/>
       <right/>
@@ -2467,11 +2616,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="80" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="293">
+  <cellXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2769,6 +2934,9 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="35" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2842,6 +3010,14 @@
     <xf numFmtId="49" fontId="24" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2861,9 +3037,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2893,16 +3066,34 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="36" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="80" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -4088,11 +4279,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="244" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="242"/>
-      <c r="D3" s="242"/>
+      <c r="C3" s="245"/>
+      <c r="D3" s="245"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4309,8 +4500,8 @@
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4334,46 +4525,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="265"/>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
+      <c r="A1" s="268"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="266" t="s">
+      <c r="G1" s="269" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="261"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="266" t="s">
+      <c r="M1" s="269" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="258"/>
-      <c r="Q1" s="259"/>
+      <c r="N1" s="261"/>
+      <c r="O1" s="261"/>
+      <c r="P1" s="261"/>
+      <c r="Q1" s="262"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="254"/>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="263"/>
+      <c r="C2" s="263"/>
+      <c r="D2" s="263"/>
+      <c r="E2" s="263"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
-      <c r="J2" s="260"/>
-      <c r="K2" s="260"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="260"/>
-      <c r="N2" s="260"/>
-      <c r="O2" s="260"/>
-      <c r="P2" s="260"/>
-      <c r="Q2" s="261"/>
+      <c r="M2" s="263"/>
+      <c r="N2" s="263"/>
+      <c r="O2" s="263"/>
+      <c r="P2" s="263"/>
+      <c r="Q2" s="264"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -4823,15 +5014,15 @@
       <c r="H15" s="63">
         <v>12.87</v>
       </c>
-      <c r="I15" s="267"/>
-      <c r="J15" s="251"/>
-      <c r="K15" s="251"/>
+      <c r="I15" s="270"/>
+      <c r="J15" s="254"/>
+      <c r="K15" s="254"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="264"/>
-      <c r="P15" s="264"/>
-      <c r="Q15" s="264"/>
+      <c r="O15" s="267"/>
+      <c r="P15" s="267"/>
+      <c r="Q15" s="267"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
@@ -4953,13 +5144,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="268" t="s">
+      <c r="A21" s="271" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="263"/>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
-      <c r="E21" s="263"/>
+      <c r="B21" s="266"/>
+      <c r="C21" s="266"/>
+      <c r="D21" s="266"/>
+      <c r="E21" s="266"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -4974,11 +5165,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="263"/>
-      <c r="B22" s="263"/>
-      <c r="C22" s="263"/>
-      <c r="D22" s="263"/>
-      <c r="E22" s="263"/>
+      <c r="A22" s="266"/>
+      <c r="B22" s="266"/>
+      <c r="C22" s="266"/>
+      <c r="D22" s="266"/>
+      <c r="E22" s="266"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -5227,10 +5418,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>9144.59</v>
       </c>
-      <c r="C33" s="252" t="s">
+      <c r="C33" s="255" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="253"/>
+      <c r="D33" s="256"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -5253,10 +5444,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>331.57</v>
       </c>
-      <c r="C34" s="252" t="s">
+      <c r="C34" s="255" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="253"/>
+      <c r="D34" s="256"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -5553,10 +5744,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="248" t="s">
+      <c r="A48" s="251" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="249"/>
+      <c r="B48" s="252"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -5739,8 +5930,8 @@
   </sheetPr>
   <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7763,8 +7954,8 @@
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7788,34 +7979,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="269" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
+      <c r="B1" s="269"/>
+      <c r="C1" s="269"/>
+      <c r="D1" s="269"/>
+      <c r="E1" s="269"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="266" t="s">
+      <c r="G1" s="269" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="259"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="262"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="269"/>
-      <c r="B2" s="269"/>
-      <c r="C2" s="269"/>
-      <c r="D2" s="269"/>
-      <c r="E2" s="269"/>
+      <c r="A2" s="272"/>
+      <c r="B2" s="272"/>
+      <c r="C2" s="272"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
-      <c r="J2" s="260"/>
-      <c r="K2" s="261"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="264"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -8120,9 +8311,9 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="264"/>
-      <c r="J15" s="264"/>
-      <c r="K15" s="264"/>
+      <c r="I15" s="267"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="127" t="s">
@@ -8226,13 +8417,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="268" t="s">
+      <c r="A21" s="271" t="s">
         <v>330</v>
       </c>
-      <c r="B21" s="263"/>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
-      <c r="E21" s="263"/>
+      <c r="B21" s="266"/>
+      <c r="C21" s="266"/>
+      <c r="D21" s="266"/>
+      <c r="E21" s="266"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -8247,11 +8438,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="263"/>
-      <c r="B22" s="263"/>
-      <c r="C22" s="263"/>
-      <c r="D22" s="263"/>
-      <c r="E22" s="263"/>
+      <c r="A22" s="266"/>
+      <c r="B22" s="266"/>
+      <c r="C22" s="266"/>
+      <c r="D22" s="266"/>
+      <c r="E22" s="266"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -8500,10 +8691,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>10076.74</v>
       </c>
-      <c r="C33" s="252" t="s">
+      <c r="C33" s="255" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="253"/>
+      <c r="D33" s="256"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -8526,10 +8717,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>337.3</v>
       </c>
-      <c r="C34" s="252" t="s">
+      <c r="C34" s="255" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="253"/>
+      <c r="D34" s="256"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -8826,10 +9017,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="248" t="s">
+      <c r="A48" s="251" t="s">
         <v>331</v>
       </c>
-      <c r="B48" s="249"/>
+      <c r="B48" s="252"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -9011,7 +9202,7 @@
   <dimension ref="A1:AZ47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10774,13 +10965,2672 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6606D7B1-0B35-6348-9F91-058959CA14D7}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W55"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.25" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="59" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="5" customWidth="1"/>
+    <col min="9" max="10" width="12.25" style="5" customWidth="1"/>
+    <col min="11" max="11" width="49.5" style="5" customWidth="1"/>
+    <col min="12" max="12" width="5.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="53.375" style="5" customWidth="1"/>
+    <col min="14" max="16" width="12.25" style="5" customWidth="1"/>
+    <col min="17" max="17" width="50.125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="12.25" style="5" customWidth="1"/>
+    <col min="19" max="19" width="54.25" style="5" customWidth="1"/>
+    <col min="20" max="20" width="14.5" style="5" customWidth="1"/>
+    <col min="21" max="22" width="12.25" style="5"/>
+    <col min="23" max="23" width="48.5" style="5" customWidth="1"/>
+    <col min="24" max="16384" width="12.25" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="269" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="269"/>
+      <c r="C1" s="269"/>
+      <c r="D1" s="269"/>
+      <c r="E1" s="269"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="269" t="s">
+        <v>361</v>
+      </c>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="262"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="269" t="s">
+        <v>362</v>
+      </c>
+      <c r="N1" s="261"/>
+      <c r="O1" s="261"/>
+      <c r="P1" s="261"/>
+      <c r="Q1" s="262"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="269" t="s">
+        <v>364</v>
+      </c>
+      <c r="T1" s="261"/>
+      <c r="U1" s="261"/>
+      <c r="V1" s="261"/>
+      <c r="W1" s="262"/>
+    </row>
+    <row r="2" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="272"/>
+      <c r="B2" s="272"/>
+      <c r="C2" s="272"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="264"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="263"/>
+      <c r="N2" s="263"/>
+      <c r="O2" s="263"/>
+      <c r="P2" s="263"/>
+      <c r="Q2" s="264"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="263"/>
+      <c r="T2" s="263"/>
+      <c r="U2" s="263"/>
+      <c r="V2" s="263"/>
+      <c r="W2" s="264"/>
+    </row>
+    <row r="3" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+    </row>
+    <row r="4" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="42">
+        <v>11643.4</v>
+      </c>
+      <c r="C4" s="43">
+        <v>210</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="H4" s="42">
+        <v>2172.04</v>
+      </c>
+      <c r="I4" s="43">
+        <v>210</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="N4" s="42">
+        <v>82952.55</v>
+      </c>
+      <c r="O4" s="43">
+        <v>210</v>
+      </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="295" t="s">
+        <v>365</v>
+      </c>
+      <c r="T4" s="42">
+        <v>50.08</v>
+      </c>
+      <c r="U4" s="43"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="124" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="45">
+        <f>B4-B6</f>
+        <v>9966.42</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="124" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5" s="45">
+        <f>H4-H6</f>
+        <v>2005.48</v>
+      </c>
+      <c r="I5" s="46"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="124" t="s">
+        <v>213</v>
+      </c>
+      <c r="N5" s="45">
+        <f>N4-N6</f>
+        <v>75661.83</v>
+      </c>
+      <c r="O5" s="46"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="302" t="s">
+        <v>366</v>
+      </c>
+      <c r="T5" s="303">
+        <v>38</v>
+      </c>
+      <c r="U5" s="46"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="293" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" s="48">
+        <v>1676.98</v>
+      </c>
+      <c r="C6" s="49">
+        <v>220</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="125" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="48">
+        <v>166.56</v>
+      </c>
+      <c r="I6" s="49">
+        <v>220</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="125" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="48">
+        <v>7290.72</v>
+      </c>
+      <c r="O6" s="49">
+        <v>220</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="300" t="s">
+        <v>367</v>
+      </c>
+      <c r="T6" s="301">
+        <f>T4*T5</f>
+        <v>1903.04</v>
+      </c>
+      <c r="U6" s="49"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+    </row>
+    <row r="7" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="52"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+    </row>
+    <row r="8" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="124" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="45">
+        <v>1828.84</v>
+      </c>
+      <c r="C8" s="54">
+        <v>230</v>
+      </c>
+      <c r="D8" s="55">
+        <f>ROUND(B5*0.1812,2)</f>
+        <v>1805.92</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="126"/>
+      <c r="G8" s="124" t="s">
+        <v>214</v>
+      </c>
+      <c r="H8" s="45">
+        <v>251.92</v>
+      </c>
+      <c r="I8" s="54">
+        <v>230</v>
+      </c>
+      <c r="J8" s="55">
+        <f>ROUND(H5*0.1812,2)</f>
+        <v>363.39</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="126"/>
+      <c r="M8" s="124" t="s">
+        <v>214</v>
+      </c>
+      <c r="N8" s="45">
+        <v>7963.01</v>
+      </c>
+      <c r="O8" s="54">
+        <v>230</v>
+      </c>
+      <c r="P8" s="55">
+        <f>ROUND(N5*0.1812,2)</f>
+        <v>13709.92</v>
+      </c>
+      <c r="Q8" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" s="126"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="125" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="48">
+        <v>240.65</v>
+      </c>
+      <c r="C9" s="54">
+        <v>225</v>
+      </c>
+      <c r="D9" s="55">
+        <f>ROUND(B6*0.1712,2)</f>
+        <v>287.10000000000002</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="126"/>
+      <c r="G9" s="125" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="48">
+        <v>23.52</v>
+      </c>
+      <c r="I9" s="54">
+        <v>225</v>
+      </c>
+      <c r="J9" s="55">
+        <f>ROUND(H6*0.1712,2)</f>
+        <v>28.52</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="126"/>
+      <c r="M9" s="125" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9" s="48">
+        <v>1248.18</v>
+      </c>
+      <c r="O9" s="54">
+        <v>225</v>
+      </c>
+      <c r="P9" s="55">
+        <f>ROUND(N6*0.1712,2)</f>
+        <v>1248.17</v>
+      </c>
+      <c r="Q9" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="R9" s="126"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="58">
+        <f>B8+B9</f>
+        <v>2069.4899999999998</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="55">
+        <f>D8+D9</f>
+        <v>2093.02</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="76"/>
+      <c r="G10" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="58">
+        <f>H8+H9</f>
+        <v>275.44</v>
+      </c>
+      <c r="I10" s="59"/>
+      <c r="J10" s="55">
+        <f>J8+J9</f>
+        <v>391.90999999999997</v>
+      </c>
+      <c r="K10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="76"/>
+      <c r="M10" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="N10" s="58">
+        <f>N8+N9</f>
+        <v>9211.19</v>
+      </c>
+      <c r="O10" s="59"/>
+      <c r="P10" s="55">
+        <f>P8+P9</f>
+        <v>14958.09</v>
+      </c>
+      <c r="Q10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="R10" s="76"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="60"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="124" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="45">
+        <f>B5-B8-B16</f>
+        <v>8137.58</v>
+      </c>
+      <c r="C12" s="49">
+        <v>245</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="124" t="s">
+        <v>215</v>
+      </c>
+      <c r="H12" s="45">
+        <f>H5-H8-H16</f>
+        <v>1751.8799999999999</v>
+      </c>
+      <c r="I12" s="49">
+        <v>245</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="123"/>
+      <c r="M12" s="124" t="s">
+        <v>215</v>
+      </c>
+      <c r="N12" s="45">
+        <f>N5-N8-N16-N15</f>
+        <v>67010.820000000007</v>
+      </c>
+      <c r="O12" s="49">
+        <v>245</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="123"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="125" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="48">
+        <f>B6-B9</f>
+        <v>1436.33</v>
+      </c>
+      <c r="C13" s="46"/>
+      <c r="D13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="125" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="48">
+        <f>H6-H9</f>
+        <v>143.04</v>
+      </c>
+      <c r="I13" s="46"/>
+      <c r="J13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="123"/>
+      <c r="M13" s="125" t="s">
+        <v>88</v>
+      </c>
+      <c r="N13" s="48">
+        <f>N6-N9</f>
+        <v>6042.54</v>
+      </c>
+      <c r="O13" s="46"/>
+      <c r="P13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="123"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="50"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+    </row>
+    <row r="15" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="127" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="63">
+        <v>0</v>
+      </c>
+      <c r="C15" s="238"/>
+      <c r="D15" s="237"/>
+      <c r="E15" s="237"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="267"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="294" t="s">
+        <v>363</v>
+      </c>
+      <c r="N15" s="63">
+        <v>688</v>
+      </c>
+      <c r="O15" s="49">
+        <v>215</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+    </row>
+    <row r="16" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="127" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="63">
+        <v>0</v>
+      </c>
+      <c r="C16" s="49">
+        <v>243</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="127" t="s">
+        <v>217</v>
+      </c>
+      <c r="H16" s="63">
+        <v>1.68</v>
+      </c>
+      <c r="I16" s="49">
+        <v>243</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="127" t="s">
+        <v>217</v>
+      </c>
+      <c r="N16" s="63">
+        <v>0</v>
+      </c>
+      <c r="O16" s="49">
+        <v>243</v>
+      </c>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+    </row>
+    <row r="17" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="128" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="66">
+        <v>1585.4</v>
+      </c>
+      <c r="C18" s="49">
+        <v>260</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="128" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="66">
+        <v>6.64</v>
+      </c>
+      <c r="I18" s="49">
+        <v>260</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="128" t="s">
+        <v>93</v>
+      </c>
+      <c r="N18" s="66">
+        <v>25754.54</v>
+      </c>
+      <c r="O18" s="49">
+        <v>260</v>
+      </c>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="123"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="271" t="s">
+        <v>357</v>
+      </c>
+      <c r="B21" s="266"/>
+      <c r="C21" s="266"/>
+      <c r="D21" s="266"/>
+      <c r="E21" s="266"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="266"/>
+      <c r="B22" s="266"/>
+      <c r="C22" s="266"/>
+      <c r="D22" s="266"/>
+      <c r="E22" s="266"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+    </row>
+    <row r="23" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="68">
+        <f>'2022'!B16</f>
+        <v>2410.52</v>
+      </c>
+      <c r="C23" s="296"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+    </row>
+    <row r="24" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="45">
+        <f>B12+H12+N12+T6</f>
+        <v>78803.319999999992</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+    </row>
+    <row r="25" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="129" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="130">
+        <f>B23+B24</f>
+        <v>81213.84</v>
+      </c>
+      <c r="C25" s="64"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+    </row>
+    <row r="26" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="72"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+    </row>
+    <row r="27" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="77"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+    </row>
+    <row r="28" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="77">
+        <f>'2022'!B13</f>
+        <v>624.14</v>
+      </c>
+      <c r="C28" s="76"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+    </row>
+    <row r="29" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="74" t="s">
+        <v>340</v>
+      </c>
+      <c r="B29" s="77">
+        <v>0</v>
+      </c>
+      <c r="C29" s="297" t="s">
+        <v>368</v>
+      </c>
+      <c r="D29" s="131"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+    </row>
+    <row r="30" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="150">
+        <f>B28+B29</f>
+        <v>624.14</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+    </row>
+    <row r="31" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="81"/>
+      <c r="B31" s="151"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+    </row>
+    <row r="32" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="83" t="s">
+        <v>334</v>
+      </c>
+      <c r="B32" s="152">
+        <f>B25-B30</f>
+        <v>80589.7</v>
+      </c>
+      <c r="C32" s="64"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+    </row>
+    <row r="33" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="91">
+        <f>ROUND((B32-60000)*0.48+1400+4225+12180,2)</f>
+        <v>27688.06</v>
+      </c>
+      <c r="C33" s="298" t="s">
+        <v>373</v>
+      </c>
+      <c r="D33" s="256"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+    </row>
+    <row r="34" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="91">
+        <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
+        <v>420.11</v>
+      </c>
+      <c r="C34" s="255" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="256"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+    </row>
+    <row r="35" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="86" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="87">
+        <v>400</v>
+      </c>
+      <c r="C35" s="64"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+    </row>
+    <row r="36" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="72"/>
+      <c r="B36" s="153"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+    </row>
+    <row r="37" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="91">
+        <f>B33+B34-B35</f>
+        <v>27708.170000000002</v>
+      </c>
+      <c r="C37" s="76"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+    </row>
+    <row r="38" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="87">
+        <f>B18+H18+N18</f>
+        <v>27346.58</v>
+      </c>
+      <c r="C38" s="64"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+    </row>
+    <row r="39" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="154">
+        <v>0.41</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+    </row>
+    <row r="40" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="53"/>
+      <c r="B40" s="155"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+    </row>
+    <row r="41" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41" s="91">
+        <f>B37-B38+B39</f>
+        <v>362.00000000000017</v>
+      </c>
+      <c r="C41" s="76"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+    </row>
+    <row r="42" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="86" t="s">
+        <v>358</v>
+      </c>
+      <c r="B42" s="87">
+        <v>3257</v>
+      </c>
+      <c r="C42" s="64"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+    </row>
+    <row r="43" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="72"/>
+      <c r="B43" s="153"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+    </row>
+    <row r="44" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="156" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="157">
+        <f>B41-B42</f>
+        <v>-2895</v>
+      </c>
+      <c r="C44" s="138"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="306" t="s">
+        <v>378</v>
+      </c>
+      <c r="F44" s="307"/>
+      <c r="G44" s="307"/>
+      <c r="H44" s="308"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+    </row>
+    <row r="45" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="61"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="304" t="s">
+        <v>377</v>
+      </c>
+      <c r="F45" s="11">
+        <f>105600/8</f>
+        <v>13200</v>
+      </c>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+    </row>
+    <row r="46" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="304" t="s">
+        <v>376</v>
+      </c>
+      <c r="F46" s="11">
+        <f>SUM(F48:F55)</f>
+        <v>69914</v>
+      </c>
+      <c r="G46" s="240">
+        <f>N4-F47</f>
+        <v>-161.44999999999709</v>
+      </c>
+      <c r="H46" s="304" t="s">
+        <v>379</v>
+      </c>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+    </row>
+    <row r="47" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="309" t="s">
+        <v>380</v>
+      </c>
+      <c r="F47" s="309">
+        <f>F45+F46</f>
+        <v>83114</v>
+      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+    </row>
+    <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="251" t="s">
+        <v>359</v>
+      </c>
+      <c r="B48" s="252"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="304" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="11">
+        <v>21457</v>
+      </c>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+    </row>
+    <row r="49" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="92" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" s="66">
+        <f>B4+H4+N4+T6</f>
+        <v>98671.03</v>
+      </c>
+      <c r="C49" s="64"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="304" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="11">
+        <v>10652</v>
+      </c>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+    </row>
+    <row r="50" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="94" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="133">
+        <f>B10+H10+N10</f>
+        <v>11556.12</v>
+      </c>
+      <c r="C50" s="64"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="304" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="11">
+        <v>5614</v>
+      </c>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+    </row>
+    <row r="51" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="133">
+        <f>B37</f>
+        <v>27708.170000000002</v>
+      </c>
+      <c r="C51" s="64"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="304" t="s">
+        <v>374</v>
+      </c>
+      <c r="F51" s="11">
+        <v>5763</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+    </row>
+    <row r="52" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="92" t="s">
+        <v>335</v>
+      </c>
+      <c r="B52" s="66">
+        <f>6025-'2022'!B19</f>
+        <v>5985.52</v>
+      </c>
+      <c r="C52" s="64"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="304" t="s">
+        <v>375</v>
+      </c>
+      <c r="F52" s="11">
+        <v>5631</v>
+      </c>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+    </row>
+    <row r="53" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="96" t="s">
+        <v>381</v>
+      </c>
+      <c r="B53" s="88"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="304" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="11">
+        <v>5618</v>
+      </c>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+    </row>
+    <row r="54" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="96"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="304" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" s="11">
+        <v>9259</v>
+      </c>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+    </row>
+    <row r="55" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="156" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="157">
+        <f>B49-B50-B51+B52+B16</f>
+        <v>65392.260000000009</v>
+      </c>
+      <c r="C55" s="76"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="305" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55" s="11">
+        <v>5920</v>
+      </c>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="M1:Q2"/>
+    <mergeCell ref="S1:W2"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G1:K2"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A21:E22"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E2908E-9B43-2D46-8AB7-D7409FBBE284}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.25" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="5" customWidth="1"/>
+    <col min="5" max="8" width="16.125" style="5" customWidth="1"/>
+    <col min="9" max="24" width="12.25" style="5" customWidth="1"/>
+    <col min="25" max="16384" width="12.25" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+    </row>
+    <row r="2" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="100">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+    </row>
+    <row r="3" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="100">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+    </row>
+    <row r="4" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="101">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="102">
+        <f>SUM(B2:B4)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+    </row>
+    <row r="7" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="158" t="s">
+        <v>337</v>
+      </c>
+      <c r="F7" s="158" t="s">
+        <v>203</v>
+      </c>
+      <c r="G7" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="158" t="s">
+        <v>202</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="159">
+        <v>0</v>
+      </c>
+      <c r="F8" s="160">
+        <f>B10</f>
+        <v>405.26</v>
+      </c>
+      <c r="G8" s="160">
+        <f>B9</f>
+        <v>71.412000000000006</v>
+      </c>
+      <c r="H8" s="240">
+        <f>B11+B12</f>
+        <v>147.46799999999999</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="100">
+        <f>B26</f>
+        <v>71.412000000000006</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="100">
+        <f>B31</f>
+        <v>405.26</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="100" t="s">
+        <v>346</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="243" t="s">
+        <v>369</v>
+      </c>
+      <c r="B11" s="100">
+        <f>150*0.6</f>
+        <v>90</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="299" t="s">
+        <v>370</v>
+      </c>
+      <c r="B12" s="101">
+        <f>95.78*0.6</f>
+        <v>57.467999999999996</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="102">
+        <f>SUM(B9:B12)</f>
+        <v>624.14</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+    </row>
+    <row r="15" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="105"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+    </row>
+    <row r="16" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="147" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="21">
+        <v>2410.52</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+    </row>
+    <row r="17" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="101"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="109">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="158" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="158" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="158" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="158" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="158" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="158" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="158" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="158" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="158" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23" s="158" t="s">
+        <v>47</v>
+      </c>
+      <c r="L23" s="158" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="158" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="C24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="D24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="E24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="F24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="G24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="H24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="I24" s="100">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="J24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="K24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="L24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="M24" s="100">
+        <v>9.9</v>
+      </c>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="110">
+        <f>SUM(B24:M24)</f>
+        <v>119.02000000000002</v>
+      </c>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="161">
+        <f>0.6*B25</f>
+        <v>71.412000000000006</v>
+      </c>
+      <c r="C26" s="112"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="100"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+    </row>
+    <row r="28" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+    </row>
+    <row r="29" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="243" t="s">
+        <v>372</v>
+      </c>
+      <c r="B29" s="100">
+        <v>384.06</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+    </row>
+    <row r="30" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="243" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="100">
+        <v>21.2</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+    </row>
+    <row r="31" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="161">
+        <f>B29+B30</f>
+        <v>405.26</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+    </row>
+    <row r="32" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A93" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A80" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -10794,11 +13644,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="285" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="280"/>
-      <c r="C1" s="281"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="287"/>
       <c r="D1" s="164"/>
       <c r="E1" s="41" t="s">
         <v>233</v>
@@ -10942,7 +13792,7 @@
       <c r="B9" s="187"/>
       <c r="C9" s="187"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="292" t="s">
+      <c r="E9" s="243" t="s">
         <v>247</v>
       </c>
       <c r="F9" s="11"/>
@@ -10966,11 +13816,11 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="282" t="s">
+      <c r="A11" s="288" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="283"/>
-      <c r="C11" s="281"/>
+      <c r="B11" s="289"/>
+      <c r="C11" s="287"/>
       <c r="D11" s="164"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -11154,11 +14004,11 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="282" t="s">
+      <c r="A23" s="288" t="s">
         <v>260</v>
       </c>
-      <c r="B23" s="283"/>
-      <c r="C23" s="281"/>
+      <c r="B23" s="289"/>
+      <c r="C23" s="287"/>
       <c r="D23" s="164"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -11434,11 +14284,11 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="284" t="s">
+      <c r="A40" s="290" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="285"/>
-      <c r="C40" s="286"/>
+      <c r="B40" s="291"/>
+      <c r="C40" s="292"/>
       <c r="D40" s="164"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -11530,13 +14380,13 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="270"/>
-      <c r="E46" s="253"/>
-      <c r="F46" s="253"/>
-      <c r="G46" s="253"/>
-      <c r="H46" s="253"/>
-      <c r="I46" s="253"/>
-      <c r="J46" s="253"/>
+      <c r="D46" s="277"/>
+      <c r="E46" s="256"/>
+      <c r="F46" s="256"/>
+      <c r="G46" s="256"/>
+      <c r="H46" s="256"/>
+      <c r="I46" s="256"/>
+      <c r="J46" s="256"/>
     </row>
     <row r="47" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="180" t="s">
@@ -11670,11 +14520,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="271" t="s">
+      <c r="A55" s="278" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="272"/>
-      <c r="C55" s="273"/>
+      <c r="B55" s="279"/>
+      <c r="C55" s="280"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -11985,10 +14835,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="274" t="s">
+      <c r="A76" s="281" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="275"/>
+      <c r="B76" s="282"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -11999,8 +14849,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="276"/>
-      <c r="B77" s="275"/>
+      <c r="A77" s="283"/>
+      <c r="B77" s="282"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -12039,10 +14889,10 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="277" t="s">
+      <c r="A80" s="273" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="278"/>
+      <c r="B80" s="284"/>
       <c r="C80" s="64"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -12053,8 +14903,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="276"/>
-      <c r="B81" s="275"/>
+      <c r="A81" s="283"/>
+      <c r="B81" s="282"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -12261,10 +15111,10 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="277" t="s">
+      <c r="A96" s="273" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="287"/>
+      <c r="B96" s="274"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -12275,8 +15125,8 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="288"/>
-      <c r="B97" s="264"/>
+      <c r="A97" s="275"/>
+      <c r="B97" s="267"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -12425,45 +15275,45 @@
       <c r="B108" s="11"/>
     </row>
     <row r="109" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="289" t="s">
+      <c r="A109" s="276" t="s">
         <v>352</v>
       </c>
-      <c r="B109" s="287"/>
+      <c r="B109" s="274"/>
     </row>
     <row r="110" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="288"/>
-      <c r="B110" s="264"/>
+      <c r="A110" s="275"/>
+      <c r="B110" s="267"/>
     </row>
     <row r="111" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="290" t="s">
+      <c r="A111" s="241" t="s">
         <v>353</v>
       </c>
       <c r="B111" s="76"/>
     </row>
     <row r="112" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="291" t="s">
+      <c r="A112" s="242" t="s">
         <v>354</v>
       </c>
       <c r="B112" s="11"/>
     </row>
     <row r="113" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="292" t="s">
+      <c r="A113" s="243" t="s">
         <v>355</v>
       </c>
       <c r="B113" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A96:B97"/>
     <mergeCell ref="A109:B110"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
     <mergeCell ref="A80:B81"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
@@ -14644,20 +17494,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="243" t="s">
+      <c r="A1" s="246" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="244"/>
-      <c r="C1" s="244"/>
-      <c r="D1" s="244"/>
-      <c r="E1" s="245"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="248"/>
     </row>
     <row r="2" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="254"/>
-      <c r="B2" s="255"/>
-      <c r="C2" s="255"/>
-      <c r="D2" s="255"/>
-      <c r="E2" s="256"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="258"/>
+      <c r="C2" s="258"/>
+      <c r="D2" s="258"/>
+      <c r="E2" s="259"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -14817,11 +17667,11 @@
       <c r="B15" s="63">
         <v>438.04</v>
       </c>
-      <c r="C15" s="250" t="s">
+      <c r="C15" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
     </row>
     <row r="16" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -14869,20 +17719,20 @@
       <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="246" t="s">
+      <c r="A21" s="249" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="247"/>
-      <c r="C21" s="247"/>
-      <c r="D21" s="247"/>
-      <c r="E21" s="247"/>
+      <c r="B21" s="250"/>
+      <c r="C21" s="250"/>
+      <c r="D21" s="250"/>
+      <c r="E21" s="250"/>
     </row>
     <row r="22" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="247"/>
-      <c r="B22" s="247"/>
-      <c r="C22" s="247"/>
-      <c r="D22" s="247"/>
-      <c r="E22" s="247"/>
+      <c r="A22" s="250"/>
+      <c r="B22" s="250"/>
+      <c r="C22" s="250"/>
+      <c r="D22" s="250"/>
+      <c r="E22" s="250"/>
     </row>
     <row r="23" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
@@ -15010,10 +17860,10 @@
         <f>ROUND((B33-18000)*0.35+1750,2)</f>
         <v>5779.41</v>
       </c>
-      <c r="C34" s="252" t="s">
+      <c r="C34" s="255" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="253"/>
+      <c r="D34" s="256"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15024,10 +17874,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>244.34</v>
       </c>
-      <c r="C35" s="252" t="s">
+      <c r="C35" s="255" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="253"/>
+      <c r="D35" s="256"/>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15154,10 +18004,10 @@
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="248" t="s">
+      <c r="A49" s="251" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="249"/>
+      <c r="B49" s="252"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -18538,34 +21388,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="265" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="257" t="s">
+      <c r="G1" s="260" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="259"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="262"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="254"/>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="263"/>
+      <c r="C2" s="263"/>
+      <c r="D2" s="263"/>
+      <c r="E2" s="263"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
-      <c r="J2" s="260"/>
-      <c r="K2" s="261"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="264"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -18864,11 +21714,11 @@
       <c r="B15" s="63">
         <v>1535.69</v>
       </c>
-      <c r="C15" s="250" t="s">
+      <c r="C15" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -18876,11 +21726,11 @@
       <c r="H15" s="63">
         <v>413.13</v>
       </c>
-      <c r="I15" s="250" t="s">
+      <c r="I15" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="251"/>
-      <c r="K15" s="251"/>
+      <c r="J15" s="254"/>
+      <c r="K15" s="254"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -18968,13 +21818,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="246" t="s">
+      <c r="A21" s="249" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="263"/>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
-      <c r="E21" s="263"/>
+      <c r="B21" s="266"/>
+      <c r="C21" s="266"/>
+      <c r="D21" s="266"/>
+      <c r="E21" s="266"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -18983,11 +21833,11 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="263"/>
-      <c r="B22" s="263"/>
-      <c r="C22" s="263"/>
-      <c r="D22" s="263"/>
-      <c r="E22" s="263"/>
+      <c r="A22" s="266"/>
+      <c r="B22" s="266"/>
+      <c r="C22" s="266"/>
+      <c r="D22" s="266"/>
+      <c r="E22" s="266"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -19188,10 +22038,10 @@
         <f>ROUND((B33-31000)*0.42+6300,2)</f>
         <v>7196.73</v>
       </c>
-      <c r="C34" s="252" t="s">
+      <c r="C34" s="255" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="253"/>
+      <c r="D34" s="256"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -19208,10 +22058,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>312.08999999999997</v>
       </c>
-      <c r="C35" s="252" t="s">
+      <c r="C35" s="255" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="253"/>
+      <c r="D35" s="256"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -19435,10 +22285,10 @@
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="248" t="s">
+      <c r="A50" s="251" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="249"/>
+      <c r="B50" s="252"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -23186,7 +26036,7 @@
   </sheetPr>
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -23210,48 +26060,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="265" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="257" t="s">
+      <c r="G1" s="260" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="261"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="257" t="s">
+      <c r="M1" s="260" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="258"/>
-      <c r="Q1" s="259"/>
+      <c r="N1" s="261"/>
+      <c r="O1" s="261"/>
+      <c r="P1" s="261"/>
+      <c r="Q1" s="262"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="254"/>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="263"/>
+      <c r="C2" s="263"/>
+      <c r="D2" s="263"/>
+      <c r="E2" s="263"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
-      <c r="J2" s="260"/>
-      <c r="K2" s="260"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="260"/>
-      <c r="N2" s="260"/>
-      <c r="O2" s="260"/>
-      <c r="P2" s="260"/>
-      <c r="Q2" s="261"/>
+      <c r="M2" s="263"/>
+      <c r="N2" s="263"/>
+      <c r="O2" s="263"/>
+      <c r="P2" s="263"/>
+      <c r="Q2" s="264"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -23689,11 +26539,11 @@
       <c r="B15" s="63">
         <v>175.89</v>
       </c>
-      <c r="C15" s="250" t="s">
+      <c r="C15" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -23701,17 +26551,17 @@
       <c r="H15" s="63">
         <v>13.93</v>
       </c>
-      <c r="I15" s="250" t="s">
+      <c r="I15" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="251"/>
-      <c r="K15" s="251"/>
+      <c r="J15" s="254"/>
+      <c r="K15" s="254"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="264"/>
-      <c r="P15" s="264"/>
-      <c r="Q15" s="264"/>
+      <c r="O15" s="267"/>
+      <c r="P15" s="267"/>
+      <c r="Q15" s="267"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -23835,13 +26685,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="246" t="s">
+      <c r="A21" s="249" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="263"/>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
-      <c r="E21" s="263"/>
+      <c r="B21" s="266"/>
+      <c r="C21" s="266"/>
+      <c r="D21" s="266"/>
+      <c r="E21" s="266"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -23856,11 +26706,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="263"/>
-      <c r="B22" s="263"/>
-      <c r="C22" s="263"/>
-      <c r="D22" s="263"/>
-      <c r="E22" s="263"/>
+      <c r="A22" s="266"/>
+      <c r="B22" s="266"/>
+      <c r="C22" s="266"/>
+      <c r="D22" s="266"/>
+      <c r="E22" s="266"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -24109,10 +26959,10 @@
         <f>ROUND((B32-31000)*0.42+6300,2)</f>
         <v>8538.18</v>
       </c>
-      <c r="C33" s="252" t="s">
+      <c r="C33" s="255" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="253"/>
+      <c r="D33" s="256"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -24135,10 +26985,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>329.36</v>
       </c>
-      <c r="C34" s="252" t="s">
+      <c r="C34" s="255" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="253"/>
+      <c r="D34" s="256"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -24416,10 +27266,10 @@
       <c r="Q46" s="11"/>
     </row>
     <row r="47" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="248" t="s">
+      <c r="A47" s="251" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="249"/>
+      <c r="B47" s="252"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
@@ -24603,7 +27453,7 @@
   </sheetPr>
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A49" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Paid Taxes for 2.Q 2023 (forget previous commit)
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EA755E-D81B-5F46-9D81-D6A90F12BA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23CAAC0-5A7A-D24D-BBB0-EC0B7E466B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26580" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="6600" windowWidth="51200" windowHeight="28300" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="384">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1141,9 +1141,6 @@
     <t>Bescheid bekommen über die Vorauszahlung für 2023. Diese ergibt 3257€ (1.Q: 814€;  2.Q: 814€;  3.Q: 814€;  4.Q: 815€), selber Betrag wie 2022, d.h dieser Betrag wird sich noch ändern sobald die Steuererklärung für 2022 gemacht wurde.</t>
   </si>
   <si>
-    <t>Am 10.02.2023 wurden 814€ überwiesen wegen 1.Q. Der Betrag für das 2.Q ist erst am 15.05 Fällig. Bis dahin habe ich eventuell schon die aktualisierte Vorausberechnung für 2023 und dann könnte man die restliche Jahressumme überweisen.</t>
-  </si>
-  <si>
     <t>Lohnzettel 2022 JKU</t>
   </si>
   <si>
@@ -1220,6 +1217,15 @@
   </si>
   <si>
     <t>Anmerkung: Die Gewinne durch ESPP werden nicht beruecksichtigt, also Netto ist noch ein bisschen mehr</t>
+  </si>
+  <si>
+    <t>Stand 26.04.2023</t>
+  </si>
+  <si>
+    <t>Am 10.02.2023 wurden 814€ überwiesen wegen 1.Q.</t>
+  </si>
+  <si>
+    <t>Am 26.04.2023 wurden 814€ überwiesen wegen 2.Q. Der Betrag für das 3.Q ist erst am 16.08 Fällig. Bis dahin habe ich eventuell schon die aktualisierte Vorausberechnung für 2023, weil bis dahin Steuererklaerung 2022 machen muss, und dann könnte man die restliche Jahressumme überweisen.</t>
   </si>
 </sst>
 </file>
@@ -2937,6 +2943,19 @@
     <xf numFmtId="49" fontId="35" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="36" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="80" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3010,6 +3029,42 @@
     <xf numFmtId="49" fontId="24" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3042,55 +3097,6 @@
     <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="80" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -4279,11 +4285,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="257" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="245"/>
-      <c r="D3" s="245"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="258"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4525,46 +4531,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="268"/>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
+      <c r="A1" s="281"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="269" t="s">
+      <c r="G1" s="282" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="261"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="269" t="s">
+      <c r="M1" s="282" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="261"/>
-      <c r="O1" s="261"/>
-      <c r="P1" s="261"/>
-      <c r="Q1" s="262"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="275"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="257"/>
-      <c r="B2" s="263"/>
-      <c r="C2" s="263"/>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="263"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="263"/>
-      <c r="N2" s="263"/>
-      <c r="O2" s="263"/>
-      <c r="P2" s="263"/>
-      <c r="Q2" s="264"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -5014,15 +5020,15 @@
       <c r="H15" s="63">
         <v>12.87</v>
       </c>
-      <c r="I15" s="270"/>
-      <c r="J15" s="254"/>
-      <c r="K15" s="254"/>
+      <c r="I15" s="283"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="267"/>
-      <c r="P15" s="267"/>
-      <c r="Q15" s="267"/>
+      <c r="O15" s="280"/>
+      <c r="P15" s="280"/>
+      <c r="Q15" s="280"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
@@ -5144,13 +5150,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="271" t="s">
+      <c r="A21" s="284" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="266"/>
-      <c r="C21" s="266"/>
-      <c r="D21" s="266"/>
-      <c r="E21" s="266"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -5165,11 +5171,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="266"/>
-      <c r="B22" s="266"/>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="266"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -5418,10 +5424,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>9144.59</v>
       </c>
-      <c r="C33" s="255" t="s">
+      <c r="C33" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="256"/>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -5444,10 +5450,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>331.57</v>
       </c>
-      <c r="C34" s="255" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="256"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -5744,10 +5750,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="251" t="s">
+      <c r="A48" s="264" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="252"/>
+      <c r="B48" s="265"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -7979,34 +7985,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="282" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="269"/>
-      <c r="C1" s="269"/>
-      <c r="D1" s="269"/>
-      <c r="E1" s="269"/>
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="269" t="s">
+      <c r="G1" s="282" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="262"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="272"/>
-      <c r="B2" s="272"/>
-      <c r="C2" s="272"/>
-      <c r="D2" s="272"/>
-      <c r="E2" s="272"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="264"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="277"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -8311,9 +8317,9 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="267"/>
-      <c r="J15" s="267"/>
-      <c r="K15" s="267"/>
+      <c r="I15" s="280"/>
+      <c r="J15" s="280"/>
+      <c r="K15" s="280"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="127" t="s">
@@ -8417,13 +8423,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="271" t="s">
+      <c r="A21" s="284" t="s">
         <v>330</v>
       </c>
-      <c r="B21" s="266"/>
-      <c r="C21" s="266"/>
-      <c r="D21" s="266"/>
-      <c r="E21" s="266"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -8438,11 +8444,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="266"/>
-      <c r="B22" s="266"/>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="266"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -8691,10 +8697,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>10076.74</v>
       </c>
-      <c r="C33" s="255" t="s">
+      <c r="C33" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="256"/>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -8717,10 +8723,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>337.3</v>
       </c>
-      <c r="C34" s="255" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="256"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -9017,10 +9023,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="251" t="s">
+      <c r="A48" s="264" t="s">
         <v>331</v>
       </c>
-      <c r="B48" s="252"/>
+      <c r="B48" s="265"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -10971,7 +10977,7 @@
   </sheetPr>
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -11000,62 +11006,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="269" t="s">
-        <v>356</v>
-      </c>
-      <c r="B1" s="269"/>
-      <c r="C1" s="269"/>
-      <c r="D1" s="269"/>
-      <c r="E1" s="269"/>
+      <c r="A1" s="282" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="269" t="s">
+      <c r="G1" s="282" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="282" t="s">
         <v>361</v>
       </c>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="262"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="269" t="s">
-        <v>362</v>
-      </c>
-      <c r="N1" s="261"/>
-      <c r="O1" s="261"/>
-      <c r="P1" s="261"/>
-      <c r="Q1" s="262"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="275"/>
       <c r="R1" s="122"/>
-      <c r="S1" s="269" t="s">
-        <v>364</v>
-      </c>
-      <c r="T1" s="261"/>
-      <c r="U1" s="261"/>
-      <c r="V1" s="261"/>
-      <c r="W1" s="262"/>
+      <c r="S1" s="282" t="s">
+        <v>363</v>
+      </c>
+      <c r="T1" s="274"/>
+      <c r="U1" s="274"/>
+      <c r="V1" s="274"/>
+      <c r="W1" s="275"/>
     </row>
     <row r="2" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="272"/>
-      <c r="B2" s="272"/>
-      <c r="C2" s="272"/>
-      <c r="D2" s="272"/>
-      <c r="E2" s="272"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="264"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="277"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="263"/>
-      <c r="N2" s="263"/>
-      <c r="O2" s="263"/>
-      <c r="P2" s="263"/>
-      <c r="Q2" s="264"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277"/>
       <c r="R2" s="122"/>
-      <c r="S2" s="263"/>
-      <c r="T2" s="263"/>
-      <c r="U2" s="263"/>
-      <c r="V2" s="263"/>
-      <c r="W2" s="264"/>
+      <c r="S2" s="276"/>
+      <c r="T2" s="276"/>
+      <c r="U2" s="276"/>
+      <c r="V2" s="276"/>
+      <c r="W2" s="277"/>
     </row>
     <row r="3" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -11125,8 +11131,8 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="295" t="s">
-        <v>365</v>
+      <c r="S4" s="246" t="s">
+        <v>364</v>
       </c>
       <c r="T4" s="42">
         <v>50.08</v>
@@ -11169,10 +11175,10 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="123"/>
-      <c r="S5" s="302" t="s">
-        <v>366</v>
-      </c>
-      <c r="T5" s="303">
+      <c r="S5" s="252" t="s">
+        <v>365</v>
+      </c>
+      <c r="T5" s="253">
         <v>38</v>
       </c>
       <c r="U5" s="46"/>
@@ -11180,8 +11186,8 @@
       <c r="W5" s="11"/>
     </row>
     <row r="6" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="293" t="s">
-        <v>360</v>
+      <c r="A6" s="244" t="s">
+        <v>359</v>
       </c>
       <c r="B6" s="48">
         <v>1676.98</v>
@@ -11216,10 +11222,10 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="123"/>
-      <c r="S6" s="300" t="s">
-        <v>367</v>
-      </c>
-      <c r="T6" s="301">
+      <c r="S6" s="250" t="s">
+        <v>366</v>
+      </c>
+      <c r="T6" s="251">
         <f>T4*T5</f>
         <v>1903.04</v>
       </c>
@@ -11584,12 +11590,12 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="267"/>
-      <c r="J15" s="267"/>
-      <c r="K15" s="267"/>
+      <c r="I15" s="280"/>
+      <c r="J15" s="280"/>
+      <c r="K15" s="280"/>
       <c r="L15" s="11"/>
-      <c r="M15" s="294" t="s">
-        <v>363</v>
+      <c r="M15" s="245" t="s">
+        <v>362</v>
       </c>
       <c r="N15" s="63">
         <v>688</v>
@@ -11766,13 +11772,13 @@
       <c r="W20" s="11"/>
     </row>
     <row r="21" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="271" t="s">
-        <v>357</v>
-      </c>
-      <c r="B21" s="266"/>
-      <c r="C21" s="266"/>
-      <c r="D21" s="266"/>
-      <c r="E21" s="266"/>
+      <c r="A21" s="284" t="s">
+        <v>356</v>
+      </c>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -11792,11 +11798,11 @@
       <c r="W21" s="11"/>
     </row>
     <row r="22" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="266"/>
-      <c r="B22" s="266"/>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="266"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -11818,7 +11824,7 @@
         <f>'2022'!B16</f>
         <v>2410.52</v>
       </c>
-      <c r="C23" s="296"/>
+      <c r="C23" s="247"/>
       <c r="D23" s="61"/>
       <c r="E23" s="61"/>
       <c r="F23" s="11"/>
@@ -11953,8 +11959,8 @@
       <c r="B29" s="77">
         <v>0</v>
       </c>
-      <c r="C29" s="297" t="s">
-        <v>368</v>
+      <c r="C29" s="248" t="s">
+        <v>367</v>
       </c>
       <c r="D29" s="131"/>
       <c r="E29" s="11"/>
@@ -12045,10 +12051,10 @@
         <f>ROUND((B32-60000)*0.48+1400+4225+12180,2)</f>
         <v>27688.06</v>
       </c>
-      <c r="C33" s="298" t="s">
-        <v>373</v>
-      </c>
-      <c r="D33" s="256"/>
+      <c r="C33" s="289" t="s">
+        <v>372</v>
+      </c>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -12071,10 +12077,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>420.11</v>
       </c>
-      <c r="C34" s="255" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="256"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -12247,7 +12253,7 @@
     </row>
     <row r="42" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="86" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B42" s="87">
         <v>3257</v>
@@ -12297,12 +12303,12 @@
       </c>
       <c r="C44" s="138"/>
       <c r="D44" s="11"/>
-      <c r="E44" s="306" t="s">
-        <v>378</v>
-      </c>
-      <c r="F44" s="307"/>
-      <c r="G44" s="307"/>
-      <c r="H44" s="308"/>
+      <c r="E44" s="286" t="s">
+        <v>377</v>
+      </c>
+      <c r="F44" s="287"/>
+      <c r="G44" s="287"/>
+      <c r="H44" s="288"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
@@ -12318,8 +12324,8 @@
       <c r="B45" s="61"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
-      <c r="E45" s="304" t="s">
-        <v>377</v>
+      <c r="E45" s="254" t="s">
+        <v>376</v>
       </c>
       <c r="F45" s="11">
         <f>105600/8</f>
@@ -12342,8 +12348,8 @@
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="304" t="s">
-        <v>376</v>
+      <c r="E46" s="254" t="s">
+        <v>375</v>
       </c>
       <c r="F46" s="11">
         <f>SUM(F48:F55)</f>
@@ -12353,8 +12359,8 @@
         <f>N4-F47</f>
         <v>-161.44999999999709</v>
       </c>
-      <c r="H46" s="304" t="s">
-        <v>379</v>
+      <c r="H46" s="254" t="s">
+        <v>378</v>
       </c>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
@@ -12371,10 +12377,10 @@
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
-      <c r="E47" s="309" t="s">
-        <v>380</v>
-      </c>
-      <c r="F47" s="309">
+      <c r="E47" s="256" t="s">
+        <v>379</v>
+      </c>
+      <c r="F47" s="256">
         <f>F45+F46</f>
         <v>83114</v>
       </c>
@@ -12391,13 +12397,13 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="251" t="s">
-        <v>359</v>
-      </c>
-      <c r="B48" s="252"/>
+      <c r="A48" s="264" t="s">
+        <v>358</v>
+      </c>
+      <c r="B48" s="265"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
-      <c r="E48" s="304" t="s">
+      <c r="E48" s="254" t="s">
         <v>42</v>
       </c>
       <c r="F48" s="11">
@@ -12425,7 +12431,7 @@
       </c>
       <c r="C49" s="64"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="304" t="s">
+      <c r="E49" s="254" t="s">
         <v>43</v>
       </c>
       <c r="F49" s="11">
@@ -12453,7 +12459,7 @@
       </c>
       <c r="C50" s="64"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="304" t="s">
+      <c r="E50" s="254" t="s">
         <v>44</v>
       </c>
       <c r="F50" s="11">
@@ -12481,8 +12487,8 @@
       </c>
       <c r="C51" s="64"/>
       <c r="D51" s="11"/>
-      <c r="E51" s="304" t="s">
-        <v>374</v>
+      <c r="E51" s="254" t="s">
+        <v>373</v>
       </c>
       <c r="F51" s="11">
         <v>5763</v>
@@ -12509,8 +12515,8 @@
       </c>
       <c r="C52" s="64"/>
       <c r="D52" s="11"/>
-      <c r="E52" s="304" t="s">
-        <v>375</v>
+      <c r="E52" s="254" t="s">
+        <v>374</v>
       </c>
       <c r="F52" s="11">
         <v>5631</v>
@@ -12529,12 +12535,12 @@
     </row>
     <row r="53" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="96" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B53" s="88"/>
       <c r="C53" s="64"/>
       <c r="D53" s="11"/>
-      <c r="E53" s="304" t="s">
+      <c r="E53" s="254" t="s">
         <v>47</v>
       </c>
       <c r="F53" s="11">
@@ -12557,7 +12563,7 @@
       <c r="B54" s="88"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
-      <c r="E54" s="304" t="s">
+      <c r="E54" s="254" t="s">
         <v>48</v>
       </c>
       <c r="F54" s="11">
@@ -12585,7 +12591,7 @@
       </c>
       <c r="C55" s="76"/>
       <c r="D55" s="11"/>
-      <c r="E55" s="305" t="s">
+      <c r="E55" s="255" t="s">
         <v>49</v>
       </c>
       <c r="F55" s="11">
@@ -12958,7 +12964,7 @@
     </row>
     <row r="11" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="243" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B11" s="100">
         <f>150*0.6</f>
@@ -12989,8 +12995,8 @@
       <c r="W11" s="11"/>
     </row>
     <row r="12" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="299" t="s">
-        <v>370</v>
+      <c r="A12" s="249" t="s">
+        <v>369</v>
       </c>
       <c r="B12" s="101">
         <f>95.78*0.6</f>
@@ -13503,7 +13509,7 @@
     </row>
     <row r="29" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="243" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B29" s="100">
         <v>384.06</v>
@@ -13532,7 +13538,7 @@
     </row>
     <row r="30" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="243" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B30" s="100">
         <v>21.2</v>
@@ -13628,10 +13634,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A80" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13644,11 +13650,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="290" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="287"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="292"/>
       <c r="D1" s="164"/>
       <c r="E1" s="41" t="s">
         <v>233</v>
@@ -13816,11 +13822,11 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="288" t="s">
+      <c r="A11" s="293" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="289"/>
-      <c r="C11" s="287"/>
+      <c r="B11" s="294"/>
+      <c r="C11" s="292"/>
       <c r="D11" s="164"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -14004,11 +14010,11 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="288" t="s">
+      <c r="A23" s="293" t="s">
         <v>260</v>
       </c>
-      <c r="B23" s="289"/>
-      <c r="C23" s="287"/>
+      <c r="B23" s="294"/>
+      <c r="C23" s="292"/>
       <c r="D23" s="164"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -14284,11 +14290,11 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="290" t="s">
+      <c r="A40" s="295" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="291"/>
-      <c r="C40" s="292"/>
+      <c r="B40" s="296"/>
+      <c r="C40" s="297"/>
       <c r="D40" s="164"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -14380,13 +14386,13 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="277"/>
-      <c r="E46" s="256"/>
-      <c r="F46" s="256"/>
-      <c r="G46" s="256"/>
-      <c r="H46" s="256"/>
-      <c r="I46" s="256"/>
-      <c r="J46" s="256"/>
+      <c r="D46" s="302"/>
+      <c r="E46" s="269"/>
+      <c r="F46" s="269"/>
+      <c r="G46" s="269"/>
+      <c r="H46" s="269"/>
+      <c r="I46" s="269"/>
+      <c r="J46" s="269"/>
     </row>
     <row r="47" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="180" t="s">
@@ -14520,11 +14526,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="278" t="s">
+      <c r="A55" s="303" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="279"/>
-      <c r="C55" s="280"/>
+      <c r="B55" s="304"/>
+      <c r="C55" s="305"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -14835,10 +14841,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="281" t="s">
+      <c r="A76" s="306" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="282"/>
+      <c r="B76" s="307"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -14849,8 +14855,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="283"/>
-      <c r="B77" s="282"/>
+      <c r="A77" s="308"/>
+      <c r="B77" s="307"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -14889,10 +14895,10 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="273" t="s">
+      <c r="A80" s="298" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="284"/>
+      <c r="B80" s="309"/>
       <c r="C80" s="64"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -14903,8 +14909,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="283"/>
-      <c r="B81" s="282"/>
+      <c r="A81" s="308"/>
+      <c r="B81" s="307"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -15111,10 +15117,10 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="273" t="s">
+      <c r="A96" s="298" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="274"/>
+      <c r="B96" s="299"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -15125,8 +15131,8 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="275"/>
-      <c r="B97" s="267"/>
+      <c r="A97" s="300"/>
+      <c r="B97" s="280"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -15275,14 +15281,14 @@
       <c r="B108" s="11"/>
     </row>
     <row r="109" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="276" t="s">
+      <c r="A109" s="301" t="s">
         <v>352</v>
       </c>
-      <c r="B109" s="274"/>
+      <c r="B109" s="299"/>
     </row>
     <row r="110" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="275"/>
-      <c r="B110" s="267"/>
+      <c r="A110" s="300"/>
+      <c r="B110" s="280"/>
     </row>
     <row r="111" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="241" t="s">
@@ -15298,22 +15304,33 @@
     </row>
     <row r="113" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="243" t="s">
-        <v>355</v>
+        <v>382</v>
       </c>
       <c r="B113" s="11"/>
+    </row>
+    <row r="114" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="230" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="243" t="s">
+        <v>383</v>
+      </c>
+      <c r="B115" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A109:B110"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A76:B77"/>
+    <mergeCell ref="A80:B81"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A96:B97"/>
-    <mergeCell ref="A109:B110"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A76:B77"/>
-    <mergeCell ref="A80:B81"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
@@ -17494,20 +17511,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="246" t="s">
+      <c r="A1" s="259" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="247"/>
-      <c r="C1" s="247"/>
-      <c r="D1" s="247"/>
-      <c r="E1" s="248"/>
+      <c r="B1" s="260"/>
+      <c r="C1" s="260"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="261"/>
     </row>
     <row r="2" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="257"/>
-      <c r="B2" s="258"/>
-      <c r="C2" s="258"/>
-      <c r="D2" s="258"/>
-      <c r="E2" s="259"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="272"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -17667,11 +17684,11 @@
       <c r="B15" s="63">
         <v>438.04</v>
       </c>
-      <c r="C15" s="253" t="s">
+      <c r="C15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="254"/>
-      <c r="E15" s="254"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
     </row>
     <row r="16" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -17719,20 +17736,20 @@
       <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="249" t="s">
+      <c r="A21" s="262" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="250"/>
-      <c r="C21" s="250"/>
-      <c r="D21" s="250"/>
-      <c r="E21" s="250"/>
+      <c r="B21" s="263"/>
+      <c r="C21" s="263"/>
+      <c r="D21" s="263"/>
+      <c r="E21" s="263"/>
     </row>
     <row r="22" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="250"/>
-      <c r="B22" s="250"/>
-      <c r="C22" s="250"/>
-      <c r="D22" s="250"/>
-      <c r="E22" s="250"/>
+      <c r="A22" s="263"/>
+      <c r="B22" s="263"/>
+      <c r="C22" s="263"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="263"/>
     </row>
     <row r="23" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
@@ -17860,10 +17877,10 @@
         <f>ROUND((B33-18000)*0.35+1750,2)</f>
         <v>5779.41</v>
       </c>
-      <c r="C34" s="255" t="s">
+      <c r="C34" s="268" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="256"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17874,10 +17891,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>244.34</v>
       </c>
-      <c r="C35" s="255" t="s">
+      <c r="C35" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="256"/>
+      <c r="D35" s="269"/>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -18004,10 +18021,10 @@
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="251" t="s">
+      <c r="A49" s="264" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="252"/>
+      <c r="B49" s="265"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -21388,34 +21405,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="278" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="260" t="s">
+      <c r="G1" s="273" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="262"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="257"/>
-      <c r="B2" s="263"/>
-      <c r="C2" s="263"/>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="264"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="277"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -21714,11 +21731,11 @@
       <c r="B15" s="63">
         <v>1535.69</v>
       </c>
-      <c r="C15" s="253" t="s">
+      <c r="C15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="254"/>
-      <c r="E15" s="254"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -21726,11 +21743,11 @@
       <c r="H15" s="63">
         <v>413.13</v>
       </c>
-      <c r="I15" s="253" t="s">
+      <c r="I15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="254"/>
-      <c r="K15" s="254"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -21818,13 +21835,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="249" t="s">
+      <c r="A21" s="262" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="266"/>
-      <c r="C21" s="266"/>
-      <c r="D21" s="266"/>
-      <c r="E21" s="266"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -21833,11 +21850,11 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="266"/>
-      <c r="B22" s="266"/>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="266"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -22038,10 +22055,10 @@
         <f>ROUND((B33-31000)*0.42+6300,2)</f>
         <v>7196.73</v>
       </c>
-      <c r="C34" s="255" t="s">
+      <c r="C34" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="256"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -22058,10 +22075,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>312.08999999999997</v>
       </c>
-      <c r="C35" s="255" t="s">
+      <c r="C35" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="256"/>
+      <c r="D35" s="269"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -22285,10 +22302,10 @@
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="251" t="s">
+      <c r="A50" s="264" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="252"/>
+      <c r="B50" s="265"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -26060,48 +26077,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="278" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="260" t="s">
+      <c r="G1" s="273" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="261"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="260" t="s">
+      <c r="M1" s="273" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="261"/>
-      <c r="O1" s="261"/>
-      <c r="P1" s="261"/>
-      <c r="Q1" s="262"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="275"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="257"/>
-      <c r="B2" s="263"/>
-      <c r="C2" s="263"/>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="263"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="263"/>
-      <c r="N2" s="263"/>
-      <c r="O2" s="263"/>
-      <c r="P2" s="263"/>
-      <c r="Q2" s="264"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -26539,11 +26556,11 @@
       <c r="B15" s="63">
         <v>175.89</v>
       </c>
-      <c r="C15" s="253" t="s">
+      <c r="C15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="254"/>
-      <c r="E15" s="254"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -26551,17 +26568,17 @@
       <c r="H15" s="63">
         <v>13.93</v>
       </c>
-      <c r="I15" s="253" t="s">
+      <c r="I15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="254"/>
-      <c r="K15" s="254"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="267"/>
-      <c r="P15" s="267"/>
-      <c r="Q15" s="267"/>
+      <c r="O15" s="280"/>
+      <c r="P15" s="280"/>
+      <c r="Q15" s="280"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -26685,13 +26702,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="249" t="s">
+      <c r="A21" s="262" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="266"/>
-      <c r="C21" s="266"/>
-      <c r="D21" s="266"/>
-      <c r="E21" s="266"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -26706,11 +26723,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="266"/>
-      <c r="B22" s="266"/>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="266"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -26959,10 +26976,10 @@
         <f>ROUND((B32-31000)*0.42+6300,2)</f>
         <v>8538.18</v>
       </c>
-      <c r="C33" s="255" t="s">
+      <c r="C33" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="256"/>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -26985,10 +27002,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>329.36</v>
       </c>
-      <c r="C34" s="255" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="256"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -27266,10 +27283,10 @@
       <c r="Q46" s="11"/>
     </row>
     <row r="47" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="251" t="s">
+      <c r="A47" s="264" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="252"/>
+      <c r="B47" s="265"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>

</xml_diff>

<commit_message>
Steuer fuer 3.Q 2023 ueberwiesen
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FB7A70-C25A-6747-8B13-FDB925962E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A728C6-9A1C-CD46-98F6-8F7BDCABB314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="6600" windowWidth="51200" windowHeight="28300" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <sheet name="2022" sheetId="16" r:id="rId15"/>
     <sheet name="Steuerkonto" sheetId="12" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="391">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1216,9 +1216,6 @@
     <t>Am 10.02.2023 wurden 814€ überwiesen wegen 1.Q.</t>
   </si>
   <si>
-    <t>Am 26.04.2023 wurden 814€ überwiesen wegen 2.Q. Der Betrag für das 3.Q ist erst am 16.08 Fällig. Bis dahin habe ich eventuell schon die aktualisierte Vorausberechnung für 2023, weil bis dahin Steuererklaerung 2022 machen muss, und dann könnte man die restliche Jahressumme überweisen.</t>
-  </si>
-  <si>
     <t>Kennzahl: 718</t>
   </si>
   <si>
@@ -1241,6 +1238,15 @@
   </si>
   <si>
     <t>Erklaerung abgegeben am 26.6.2023. Warten auf Antwort vom Finanzamt. Eigentlich sollte ich die Gutschrift von 3036 erhalten</t>
+  </si>
+  <si>
+    <t>Stand 10.08.2023</t>
+  </si>
+  <si>
+    <t>Am 26.04.2023 wurden 814€ überwiesen wegen 2.Q.</t>
+  </si>
+  <si>
+    <t>Am 10.08.2023 wurden 814€ überwiesen wegen 3.Q. Der Betrag für das 4.Q ist erst am 15.11 Fällig. Bis dahin habe ich eventuell schon die aktualisierte Vorausberechnung für 2023, weil die Steuererklaerung 2022 schon abgegeben worden ist</t>
   </si>
 </sst>
 </file>
@@ -2970,6 +2976,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="16" borderId="80" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3055,6 +3062,38 @@
     <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3079,39 +3118,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -4300,11 +4306,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="256" t="s">
+      <c r="B3" s="257" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="257"/>
-      <c r="D3" s="257"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="258"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4546,46 +4552,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="280"/>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
+      <c r="A1" s="281"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="281" t="s">
+      <c r="G1" s="282" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="273"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="281" t="s">
+      <c r="M1" s="282" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="273"/>
-      <c r="O1" s="273"/>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="275"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="269"/>
-      <c r="B2" s="275"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="275"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="275"/>
-      <c r="N2" s="275"/>
-      <c r="O2" s="275"/>
-      <c r="P2" s="275"/>
-      <c r="Q2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -5035,15 +5041,15 @@
       <c r="H15" s="63">
         <v>12.87</v>
       </c>
-      <c r="I15" s="282"/>
-      <c r="J15" s="266"/>
-      <c r="K15" s="266"/>
+      <c r="I15" s="283"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="279"/>
-      <c r="P15" s="279"/>
-      <c r="Q15" s="279"/>
+      <c r="O15" s="280"/>
+      <c r="P15" s="280"/>
+      <c r="Q15" s="280"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
@@ -5165,13 +5171,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="283" t="s">
+      <c r="A21" s="284" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -5186,11 +5192,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="278"/>
-      <c r="B22" s="278"/>
-      <c r="C22" s="278"/>
-      <c r="D22" s="278"/>
-      <c r="E22" s="278"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -5439,10 +5445,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>9144.59</v>
       </c>
-      <c r="C33" s="267" t="s">
+      <c r="C33" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="268"/>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -5465,10 +5471,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>331.57</v>
       </c>
-      <c r="C34" s="267" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="268"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -5765,10 +5771,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="263" t="s">
+      <c r="A48" s="264" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="264"/>
+      <c r="B48" s="265"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -8000,34 +8006,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="282" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="281" t="s">
+      <c r="G1" s="282" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="276"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="277"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -8332,9 +8338,9 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="279"/>
-      <c r="J15" s="279"/>
-      <c r="K15" s="279"/>
+      <c r="I15" s="280"/>
+      <c r="J15" s="280"/>
+      <c r="K15" s="280"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="127" t="s">
@@ -8438,13 +8444,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="283" t="s">
+      <c r="A21" s="284" t="s">
         <v>330</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -8459,11 +8465,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="278"/>
-      <c r="B22" s="278"/>
-      <c r="C22" s="278"/>
-      <c r="D22" s="278"/>
-      <c r="E22" s="278"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -8712,10 +8718,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>10076.74</v>
       </c>
-      <c r="C33" s="267" t="s">
+      <c r="C33" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="268"/>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -8738,10 +8744,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>337.3</v>
       </c>
-      <c r="C34" s="267" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="268"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -9038,10 +9044,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="263" t="s">
+      <c r="A48" s="264" t="s">
         <v>331</v>
       </c>
-      <c r="B48" s="264"/>
+      <c r="B48" s="265"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -11021,62 +11027,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="282" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="281" t="s">
+      <c r="G1" s="282" t="s">
         <v>360</v>
       </c>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="281" t="s">
+      <c r="M1" s="282" t="s">
         <v>361</v>
       </c>
-      <c r="N1" s="273"/>
-      <c r="O1" s="273"/>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="275"/>
       <c r="R1" s="122"/>
-      <c r="S1" s="281" t="s">
+      <c r="S1" s="282" t="s">
         <v>363</v>
       </c>
-      <c r="T1" s="273"/>
-      <c r="U1" s="273"/>
-      <c r="V1" s="273"/>
-      <c r="W1" s="274"/>
+      <c r="T1" s="274"/>
+      <c r="U1" s="274"/>
+      <c r="V1" s="274"/>
+      <c r="W1" s="275"/>
     </row>
     <row r="2" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="276"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="277"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="275"/>
-      <c r="N2" s="275"/>
-      <c r="O2" s="275"/>
-      <c r="P2" s="275"/>
-      <c r="Q2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277"/>
       <c r="R2" s="122"/>
-      <c r="S2" s="275"/>
-      <c r="T2" s="275"/>
-      <c r="U2" s="275"/>
-      <c r="V2" s="275"/>
-      <c r="W2" s="276"/>
+      <c r="S2" s="276"/>
+      <c r="T2" s="276"/>
+      <c r="U2" s="276"/>
+      <c r="V2" s="276"/>
+      <c r="W2" s="277"/>
     </row>
     <row r="3" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -11605,9 +11611,9 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="279"/>
-      <c r="J15" s="279"/>
-      <c r="K15" s="279"/>
+      <c r="I15" s="280"/>
+      <c r="J15" s="280"/>
+      <c r="K15" s="280"/>
       <c r="L15" s="11"/>
       <c r="M15" s="245" t="s">
         <v>362</v>
@@ -11787,13 +11793,13 @@
       <c r="W20" s="11"/>
     </row>
     <row r="21" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="283" t="s">
+      <c r="A21" s="284" t="s">
         <v>356</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -11813,11 +11819,11 @@
       <c r="W21" s="11"/>
     </row>
     <row r="22" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="278"/>
-      <c r="B22" s="278"/>
-      <c r="C22" s="278"/>
-      <c r="D22" s="278"/>
-      <c r="E22" s="278"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -11945,7 +11951,7 @@
     </row>
     <row r="28" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="79" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B28" s="150">
         <f>'2022'!B14</f>
@@ -12017,10 +12023,10 @@
         <f>ROUND((B30-60000)*0.48+1400+4225+12180,2)</f>
         <v>27569.02</v>
       </c>
-      <c r="C31" s="288" t="s">
+      <c r="C31" s="289" t="s">
         <v>370</v>
       </c>
-      <c r="D31" s="268"/>
+      <c r="D31" s="269"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -12043,10 +12049,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>420.11</v>
       </c>
-      <c r="C32" s="267" t="s">
+      <c r="C32" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="268"/>
+      <c r="D32" s="269"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -12063,7 +12069,7 @@
     </row>
     <row r="33" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="86" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B33" s="87">
         <f>400+21.33</f>
@@ -12268,16 +12274,16 @@
         <f>B39-B40</f>
         <v>-3036.0000000000023</v>
       </c>
-      <c r="C42" s="309" t="s">
-        <v>388</v>
+      <c r="C42" s="256" t="s">
+        <v>387</v>
       </c>
       <c r="D42" s="11"/>
-      <c r="E42" s="285" t="s">
+      <c r="E42" s="286" t="s">
         <v>375</v>
       </c>
-      <c r="F42" s="286"/>
-      <c r="G42" s="286"/>
-      <c r="H42" s="287"/>
+      <c r="F42" s="287"/>
+      <c r="G42" s="287"/>
+      <c r="H42" s="288"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
@@ -12329,7 +12335,7 @@
         <v>-161.44999999999709</v>
       </c>
       <c r="H44" s="253" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
@@ -12355,7 +12361,7 @@
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="253" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
@@ -12368,10 +12374,10 @@
       <c r="Q45" s="11"/>
     </row>
     <row r="46" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="263" t="s">
+      <c r="A46" s="264" t="s">
         <v>358</v>
       </c>
-      <c r="B46" s="264"/>
+      <c r="B46" s="265"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
       <c r="E46" s="253" t="s">
@@ -12935,7 +12941,7 @@
     </row>
     <row r="11" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="243" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B11" s="100">
         <f>150*0.6</f>
@@ -12999,14 +13005,14 @@
     </row>
     <row r="13" spans="1:23" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="248" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B13" s="101">
         <f>248</f>
         <v>248</v>
       </c>
       <c r="C13" s="243" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -13637,10 +13643,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13653,11 +13659,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="289" t="s">
+      <c r="A1" s="302" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="291"/>
+      <c r="B1" s="303"/>
+      <c r="C1" s="304"/>
       <c r="D1" s="164"/>
       <c r="E1" s="41" t="s">
         <v>233</v>
@@ -13825,11 +13831,11 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="292" t="s">
+      <c r="A11" s="305" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="293"/>
-      <c r="C11" s="291"/>
+      <c r="B11" s="306"/>
+      <c r="C11" s="304"/>
       <c r="D11" s="164"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -14013,11 +14019,11 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="292" t="s">
+      <c r="A23" s="305" t="s">
         <v>260</v>
       </c>
-      <c r="B23" s="293"/>
-      <c r="C23" s="291"/>
+      <c r="B23" s="306"/>
+      <c r="C23" s="304"/>
       <c r="D23" s="164"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -14293,11 +14299,11 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="294" t="s">
+      <c r="A40" s="307" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="295"/>
-      <c r="C40" s="296"/>
+      <c r="B40" s="308"/>
+      <c r="C40" s="309"/>
       <c r="D40" s="164"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -14389,13 +14395,13 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="301"/>
-      <c r="E46" s="268"/>
-      <c r="F46" s="268"/>
-      <c r="G46" s="268"/>
-      <c r="H46" s="268"/>
-      <c r="I46" s="268"/>
-      <c r="J46" s="268"/>
+      <c r="D46" s="293"/>
+      <c r="E46" s="269"/>
+      <c r="F46" s="269"/>
+      <c r="G46" s="269"/>
+      <c r="H46" s="269"/>
+      <c r="I46" s="269"/>
+      <c r="J46" s="269"/>
     </row>
     <row r="47" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="180" t="s">
@@ -14529,11 +14535,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="302" t="s">
+      <c r="A55" s="294" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="303"/>
-      <c r="C55" s="304"/>
+      <c r="B55" s="295"/>
+      <c r="C55" s="296"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -14844,10 +14850,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="305" t="s">
+      <c r="A76" s="297" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="306"/>
+      <c r="B76" s="298"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -14858,8 +14864,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="307"/>
-      <c r="B77" s="306"/>
+      <c r="A77" s="299"/>
+      <c r="B77" s="298"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -14898,10 +14904,10 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="297" t="s">
+      <c r="A80" s="300" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="308"/>
+      <c r="B80" s="301"/>
       <c r="C80" s="64"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -14912,8 +14918,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="307"/>
-      <c r="B81" s="306"/>
+      <c r="A81" s="299"/>
+      <c r="B81" s="298"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -15120,10 +15126,10 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="297" t="s">
+      <c r="A96" s="300" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="298"/>
+      <c r="B96" s="291"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -15134,8 +15140,8 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="299"/>
-      <c r="B97" s="279"/>
+      <c r="A97" s="292"/>
+      <c r="B97" s="280"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -15284,14 +15290,14 @@
       <c r="B108" s="11"/>
     </row>
     <row r="109" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="300" t="s">
+      <c r="A109" s="290" t="s">
         <v>352</v>
       </c>
-      <c r="B109" s="298"/>
+      <c r="B109" s="291"/>
     </row>
     <row r="110" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="299"/>
-      <c r="B110" s="279"/>
+      <c r="A110" s="292"/>
+      <c r="B110" s="280"/>
     </row>
     <row r="111" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="241" t="s">
@@ -15318,22 +15324,32 @@
     </row>
     <row r="115" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="243" t="s">
-        <v>380</v>
-      </c>
-      <c r="B115" s="11"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="230" t="s">
+        <v>388</v>
+      </c>
+      <c r="B116" s="11"/>
+    </row>
+    <row r="117" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="243" t="s">
+        <v>390</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A96:B97"/>
     <mergeCell ref="A109:B110"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
     <mergeCell ref="A80:B81"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A96:B97"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
@@ -17514,20 +17530,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="259" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="260"/>
+      <c r="B1" s="260"/>
+      <c r="C1" s="260"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="261"/>
     </row>
     <row r="2" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="269"/>
-      <c r="B2" s="270"/>
-      <c r="C2" s="270"/>
-      <c r="D2" s="270"/>
-      <c r="E2" s="271"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="272"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -17687,11 +17703,11 @@
       <c r="B15" s="63">
         <v>438.04</v>
       </c>
-      <c r="C15" s="265" t="s">
+      <c r="C15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="266"/>
-      <c r="E15" s="266"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
     </row>
     <row r="16" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -17739,20 +17755,20 @@
       <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="261" t="s">
+      <c r="A21" s="262" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="262"/>
-      <c r="C21" s="262"/>
-      <c r="D21" s="262"/>
-      <c r="E21" s="262"/>
+      <c r="B21" s="263"/>
+      <c r="C21" s="263"/>
+      <c r="D21" s="263"/>
+      <c r="E21" s="263"/>
     </row>
     <row r="22" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="262"/>
-      <c r="B22" s="262"/>
-      <c r="C22" s="262"/>
-      <c r="D22" s="262"/>
-      <c r="E22" s="262"/>
+      <c r="A22" s="263"/>
+      <c r="B22" s="263"/>
+      <c r="C22" s="263"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="263"/>
     </row>
     <row r="23" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
@@ -17880,10 +17896,10 @@
         <f>ROUND((B33-18000)*0.35+1750,2)</f>
         <v>5779.41</v>
       </c>
-      <c r="C34" s="267" t="s">
+      <c r="C34" s="268" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="268"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17894,10 +17910,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>244.34</v>
       </c>
-      <c r="C35" s="267" t="s">
+      <c r="C35" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="268"/>
+      <c r="D35" s="269"/>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -18024,10 +18040,10 @@
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="263" t="s">
+      <c r="A49" s="264" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="264"/>
+      <c r="B49" s="265"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -21408,34 +21424,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="278" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="272" t="s">
+      <c r="G1" s="273" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="269"/>
-      <c r="B2" s="275"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="276"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="277"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -21734,11 +21750,11 @@
       <c r="B15" s="63">
         <v>1535.69</v>
       </c>
-      <c r="C15" s="265" t="s">
+      <c r="C15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="266"/>
-      <c r="E15" s="266"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -21746,11 +21762,11 @@
       <c r="H15" s="63">
         <v>413.13</v>
       </c>
-      <c r="I15" s="265" t="s">
+      <c r="I15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="266"/>
-      <c r="K15" s="266"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -21838,13 +21854,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="261" t="s">
+      <c r="A21" s="262" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -21853,11 +21869,11 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="278"/>
-      <c r="B22" s="278"/>
-      <c r="C22" s="278"/>
-      <c r="D22" s="278"/>
-      <c r="E22" s="278"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -22058,10 +22074,10 @@
         <f>ROUND((B33-31000)*0.42+6300,2)</f>
         <v>7196.73</v>
       </c>
-      <c r="C34" s="267" t="s">
+      <c r="C34" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="268"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -22078,10 +22094,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>312.08999999999997</v>
       </c>
-      <c r="C35" s="267" t="s">
+      <c r="C35" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="268"/>
+      <c r="D35" s="269"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -22305,10 +22321,10 @@
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="263" t="s">
+      <c r="A50" s="264" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="264"/>
+      <c r="B50" s="265"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -26080,48 +26096,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="278" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="272" t="s">
+      <c r="G1" s="273" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="273"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="272" t="s">
+      <c r="M1" s="273" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="273"/>
-      <c r="O1" s="273"/>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="275"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="269"/>
-      <c r="B2" s="275"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="275"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="275"/>
-      <c r="N2" s="275"/>
-      <c r="O2" s="275"/>
-      <c r="P2" s="275"/>
-      <c r="Q2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -26559,11 +26575,11 @@
       <c r="B15" s="63">
         <v>175.89</v>
       </c>
-      <c r="C15" s="265" t="s">
+      <c r="C15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="266"/>
-      <c r="E15" s="266"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -26571,17 +26587,17 @@
       <c r="H15" s="63">
         <v>13.93</v>
       </c>
-      <c r="I15" s="265" t="s">
+      <c r="I15" s="266" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="266"/>
-      <c r="K15" s="266"/>
+      <c r="J15" s="267"/>
+      <c r="K15" s="267"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="279"/>
-      <c r="P15" s="279"/>
-      <c r="Q15" s="279"/>
+      <c r="O15" s="280"/>
+      <c r="P15" s="280"/>
+      <c r="Q15" s="280"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -26705,13 +26721,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="261" t="s">
+      <c r="A21" s="262" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -26726,11 +26742,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="278"/>
-      <c r="B22" s="278"/>
-      <c r="C22" s="278"/>
-      <c r="D22" s="278"/>
-      <c r="E22" s="278"/>
+      <c r="A22" s="279"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -26979,10 +26995,10 @@
         <f>ROUND((B32-31000)*0.42+6300,2)</f>
         <v>8538.18</v>
       </c>
-      <c r="C33" s="267" t="s">
+      <c r="C33" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="268"/>
+      <c r="D33" s="269"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -27005,10 +27021,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>329.36</v>
       </c>
-      <c r="C34" s="267" t="s">
+      <c r="C34" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="268"/>
+      <c r="D34" s="269"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -27286,10 +27302,10 @@
       <c r="Q46" s="11"/>
     </row>
     <row r="47" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="263" t="s">
+      <c r="A47" s="264" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="264"/>
+      <c r="B47" s="265"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>

</xml_diff>

<commit_message>
Gutschrift einkommensteuererklärung 2023 erhalten
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c_pre\Documents\Git Finance\Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518D35AE-81A1-4B20-B9E3-5862CD4C22E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FF5DDC-11E4-458C-999B-2803310FBB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="425">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1311,9 +1311,6 @@
     <t>Wintersemester 2023/2024</t>
   </si>
   <si>
-    <t>Juni (mit Ulraubsgeld)</t>
-  </si>
-  <si>
     <t>November (mit Weihnachtsgeld)</t>
   </si>
   <si>
@@ -1323,9 +1320,6 @@
     <t>Apple Fulltime: Gross Pay (, inkludiert Urlaubs/Weihnachtsgeld + Performance bonus, in Euro)</t>
   </si>
   <si>
-    <t>Nebenrechnung um zu checken ob im Jahresbruttogehalt die RSUs enthalten sind =&gt; JA</t>
-  </si>
-  <si>
     <t>Pendlereuro</t>
   </si>
   <si>
@@ -1333,6 +1327,30 @@
   </si>
   <si>
     <t>weniger als 730€, somit bleibt dieser Zuverdienst steuerfrei =&gt; ich müsste keine Steuererklärung mehr abgeben</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>Stand 24.06.2024</t>
+  </si>
+  <si>
+    <t>Steuererklärung für 2023 (eingereicht am 16.6.2024) ergab eine Gutschrift von 925€ =&gt; wurde auf SteuerKonto überwiesen. Rückerstatttung von die 925€ wurde sofort beantragt.</t>
+  </si>
+  <si>
+    <t>Stand 25.06.2024</t>
+  </si>
+  <si>
+    <t>Rückerstatttung von 925€ wurde überwiesen =&gt; Kontostand auf 0€</t>
+  </si>
+  <si>
+    <t>Gutschrift von 925€ erhalten am 17.6.2024 =&gt; DONE</t>
+  </si>
+  <si>
+    <t>Juni (mit Urlaubsgeld)</t>
+  </si>
+  <si>
+    <t>Nebenrechnung um zu checken ob im Jahresbruttogehalt die RSUs enthalten sind =&gt; JA sind enthalten, weil ca gleich mit Jahresbrutto (KZ210)</t>
   </si>
 </sst>
 </file>
@@ -2763,7 +2781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="16" borderId="80" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="316">
+  <cellXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3168,11 +3186,14 @@
     <xf numFmtId="49" fontId="36" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3192,9 +3213,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3223,6 +3241,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -13743,8 +13770,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.26953125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -13886,7 +13913,7 @@
     </row>
     <row r="12" spans="1:6" ht="21.95" customHeight="1">
       <c r="A12" s="124" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="B12" s="45">
         <f>B5-B8-B16-B15</f>
@@ -14135,9 +14162,7 @@
         <v>442.33</v>
       </c>
       <c r="C33" s="64"/>
-      <c r="D33" s="11" t="s">
-        <v>404</v>
-      </c>
+      <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
     </row>
@@ -14236,20 +14261,22 @@
         <f>B39-B40</f>
         <v>-924.99999999999625</v>
       </c>
-      <c r="C42" s="256" t="s">
+      <c r="C42" s="316" t="s">
         <v>408</v>
       </c>
-      <c r="D42" s="11"/>
+      <c r="D42" s="317"/>
       <c r="E42" s="292" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="F42" s="293"/>
     </row>
     <row r="43" spans="1:8" ht="21.95" customHeight="1">
       <c r="A43" s="61"/>
       <c r="B43" s="61"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="C43" s="318" t="s">
+        <v>422</v>
+      </c>
+      <c r="D43" s="289"/>
       <c r="E43" s="253" t="s">
         <v>374</v>
       </c>
@@ -14264,7 +14291,7 @@
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="253" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F44" s="258">
         <f>SUM(F46:F51)+SUM(H46:H51)</f>
@@ -14367,7 +14394,7 @@
         <v>5824</v>
       </c>
       <c r="G49" s="253" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H49" s="258">
         <v>11353</v>
@@ -14390,7 +14417,7 @@
         <v>6170</v>
       </c>
       <c r="G50" s="253" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H50" s="258">
         <v>12340</v>
@@ -14404,7 +14431,7 @@
       <c r="C51" s="64"/>
       <c r="D51" s="11"/>
       <c r="E51" s="253" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="F51" s="258">
         <v>12530</v>
@@ -14438,13 +14465,15 @@
       <c r="F53" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A21:E22"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -14462,8 +14491,8 @@
   </sheetPr>
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.26953125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -14942,16 +14971,19 @@
     </row>
     <row r="16" spans="1:23" ht="22.35" customHeight="1">
       <c r="A16" s="248" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B16" s="101">
         <f>21.33</f>
         <v>21.33</v>
       </c>
       <c r="C16" s="243" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D16" s="11"/>
+      <c r="E16" s="5" t="s">
+        <v>404</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -15008,7 +15040,7 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -15526,10 +15558,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A99" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.26953125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -16278,7 +16310,7 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="299"/>
+      <c r="D46" s="300"/>
       <c r="E46" s="275"/>
       <c r="F46" s="275"/>
       <c r="G46" s="275"/>
@@ -16418,11 +16450,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.35" customHeight="1">
-      <c r="A55" s="300" t="s">
+      <c r="A55" s="301" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="301"/>
-      <c r="C55" s="302"/>
+      <c r="B55" s="302"/>
+      <c r="C55" s="303"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -16733,10 +16765,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.35" customHeight="1">
-      <c r="A76" s="303" t="s">
+      <c r="A76" s="304" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="304"/>
+      <c r="B76" s="305"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -16747,8 +16779,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.35" customHeight="1">
-      <c r="A77" s="305"/>
-      <c r="B77" s="304"/>
+      <c r="A77" s="306"/>
+      <c r="B77" s="305"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -16787,7 +16819,7 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.35" customHeight="1">
-      <c r="A80" s="306" t="s">
+      <c r="A80" s="296" t="s">
         <v>307</v>
       </c>
       <c r="B80" s="307"/>
@@ -16801,8 +16833,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.35" customHeight="1">
-      <c r="A81" s="305"/>
-      <c r="B81" s="304"/>
+      <c r="A81" s="306"/>
+      <c r="B81" s="305"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -17009,7 +17041,7 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.35" customHeight="1">
-      <c r="A96" s="306" t="s">
+      <c r="A96" s="296" t="s">
         <v>322</v>
       </c>
       <c r="B96" s="297"/>
@@ -17173,7 +17205,7 @@
       <c r="B108" s="11"/>
     </row>
     <row r="109" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A109" s="296" t="s">
+      <c r="A109" s="299" t="s">
         <v>352</v>
       </c>
       <c r="B109" s="297"/>
@@ -17251,19 +17283,47 @@
         <v>396</v>
       </c>
     </row>
+    <row r="124" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A124" s="296" t="s">
+        <v>417</v>
+      </c>
+      <c r="B124" s="297"/>
+    </row>
+    <row r="125" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A125" s="298"/>
+      <c r="B125" s="286"/>
+    </row>
+    <row r="126" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A126" s="230" t="s">
+        <v>418</v>
+      </c>
+      <c r="B126" s="76" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A127" s="230" t="s">
+        <v>420</v>
+      </c>
+      <c r="B127" s="76" t="s">
+        <v>421</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A96:B97"/>
+    <mergeCell ref="A124:B125"/>
     <mergeCell ref="A109:B110"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
     <mergeCell ref="A80:B81"/>
   </mergeCells>
+  <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Fixed Income auschuettung (1833.6euro)
</commit_message>
<xml_diff>
--- a/Einkommenssteuerberechnungen.xlsx
+++ b/Einkommenssteuerberechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preissl/Documents/Private/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE3A7C8-32BA-6E40-8176-3F8529E0DFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126A2BF5-D93C-124F-9D19-17D8133B7D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="50880" windowHeight="26800" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="446">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1398,6 +1398,24 @@
   </si>
   <si>
     <t>Erklaerung abgegeben am 10.04.2025</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Stand 10.04.2025</t>
+  </si>
+  <si>
+    <t>Steuererklärung für 2024 ergab eine Gutschrift von 646€ =&gt; wurde auf SteuerKonto überwiesen. Rückerstatttung von die 646€ wurde sofort beantragt.</t>
+  </si>
+  <si>
+    <t>Gutschrift von 646€ erhalten am 22.4.2025 =&gt; DONE</t>
+  </si>
+  <si>
+    <t>Stand 15.04.2024</t>
+  </si>
+  <si>
+    <t>Rückerstatttung von 646€ wurde überwiesen =&gt; Kontostand auf 0€</t>
   </si>
 </sst>
 </file>
@@ -2855,7 +2873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="16" borderId="80" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="328">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3182,6 +3200,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3273,8 +3293,32 @@
     <xf numFmtId="49" fontId="36" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3307,30 +3351,6 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4520,11 +4540,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="270" t="s">
+      <c r="B3" s="272" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="271"/>
-      <c r="D3" s="271"/>
+      <c r="C3" s="273"/>
+      <c r="D3" s="273"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4766,46 +4786,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="294"/>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
+      <c r="A1" s="296"/>
+      <c r="B1" s="289"/>
+      <c r="C1" s="289"/>
+      <c r="D1" s="289"/>
+      <c r="E1" s="289"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="295" t="s">
+      <c r="G1" s="297" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="287"/>
-      <c r="K1" s="287"/>
+      <c r="H1" s="289"/>
+      <c r="I1" s="289"/>
+      <c r="J1" s="289"/>
+      <c r="K1" s="289"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="295" t="s">
+      <c r="M1" s="297" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="287"/>
-      <c r="O1" s="287"/>
-      <c r="P1" s="287"/>
-      <c r="Q1" s="288"/>
+      <c r="N1" s="289"/>
+      <c r="O1" s="289"/>
+      <c r="P1" s="289"/>
+      <c r="Q1" s="290"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="283"/>
-      <c r="B2" s="289"/>
-      <c r="C2" s="289"/>
-      <c r="D2" s="289"/>
-      <c r="E2" s="289"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="291"/>
+      <c r="C2" s="291"/>
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="289"/>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289"/>
-      <c r="J2" s="289"/>
-      <c r="K2" s="289"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="291"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="289"/>
-      <c r="N2" s="289"/>
-      <c r="O2" s="289"/>
-      <c r="P2" s="289"/>
-      <c r="Q2" s="290"/>
+      <c r="M2" s="291"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
+      <c r="Q2" s="292"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -5255,15 +5275,15 @@
       <c r="H15" s="63">
         <v>12.87</v>
       </c>
-      <c r="I15" s="296"/>
-      <c r="J15" s="280"/>
-      <c r="K15" s="280"/>
+      <c r="I15" s="298"/>
+      <c r="J15" s="282"/>
+      <c r="K15" s="282"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="293"/>
-      <c r="P15" s="293"/>
-      <c r="Q15" s="293"/>
+      <c r="O15" s="295"/>
+      <c r="P15" s="295"/>
+      <c r="Q15" s="295"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
@@ -5385,13 +5405,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="297" t="s">
+      <c r="A21" s="299" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -5406,11 +5426,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -5659,10 +5679,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>9144.59</v>
       </c>
-      <c r="C33" s="281" t="s">
+      <c r="C33" s="283" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="282"/>
+      <c r="D33" s="284"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -5685,10 +5705,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>331.57</v>
       </c>
-      <c r="C34" s="281" t="s">
+      <c r="C34" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="282"/>
+      <c r="D34" s="284"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -5985,10 +6005,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="277" t="s">
+      <c r="A48" s="279" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="278"/>
+      <c r="B48" s="280"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -8220,34 +8240,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="297" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="295" t="s">
+      <c r="G1" s="297" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="287"/>
-      <c r="K1" s="288"/>
+      <c r="H1" s="289"/>
+      <c r="I1" s="289"/>
+      <c r="J1" s="289"/>
+      <c r="K1" s="290"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="298"/>
-      <c r="B2" s="298"/>
-      <c r="C2" s="298"/>
-      <c r="D2" s="298"/>
-      <c r="E2" s="298"/>
+      <c r="A2" s="300"/>
+      <c r="B2" s="300"/>
+      <c r="C2" s="300"/>
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="289"/>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289"/>
-      <c r="J2" s="289"/>
-      <c r="K2" s="290"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="292"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -8552,9 +8572,9 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="293"/>
-      <c r="J15" s="293"/>
-      <c r="K15" s="293"/>
+      <c r="I15" s="295"/>
+      <c r="J15" s="295"/>
+      <c r="K15" s="295"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="127" t="s">
@@ -8658,13 +8678,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="297" t="s">
+      <c r="A21" s="299" t="s">
         <v>330</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -8679,11 +8699,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -8932,10 +8952,10 @@
         <f>ROUND((B32-31000)*0.42+5950,2)</f>
         <v>10076.74</v>
       </c>
-      <c r="C33" s="281" t="s">
+      <c r="C33" s="283" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="282"/>
+      <c r="D33" s="284"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -8958,10 +8978,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>337.3</v>
       </c>
-      <c r="C34" s="281" t="s">
+      <c r="C34" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="282"/>
+      <c r="D34" s="284"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -9258,10 +9278,10 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="277" t="s">
+      <c r="A48" s="279" t="s">
         <v>331</v>
       </c>
-      <c r="B48" s="278"/>
+      <c r="B48" s="280"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -11241,62 +11261,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="297" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="295" t="s">
+      <c r="G1" s="297" t="s">
         <v>360</v>
       </c>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="287"/>
-      <c r="K1" s="288"/>
+      <c r="H1" s="289"/>
+      <c r="I1" s="289"/>
+      <c r="J1" s="289"/>
+      <c r="K1" s="290"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="295" t="s">
+      <c r="M1" s="297" t="s">
         <v>361</v>
       </c>
-      <c r="N1" s="287"/>
-      <c r="O1" s="287"/>
-      <c r="P1" s="287"/>
-      <c r="Q1" s="288"/>
+      <c r="N1" s="289"/>
+      <c r="O1" s="289"/>
+      <c r="P1" s="289"/>
+      <c r="Q1" s="290"/>
       <c r="R1" s="122"/>
-      <c r="S1" s="295" t="s">
+      <c r="S1" s="297" t="s">
         <v>363</v>
       </c>
-      <c r="T1" s="287"/>
-      <c r="U1" s="287"/>
-      <c r="V1" s="287"/>
-      <c r="W1" s="288"/>
+      <c r="T1" s="289"/>
+      <c r="U1" s="289"/>
+      <c r="V1" s="289"/>
+      <c r="W1" s="290"/>
     </row>
     <row r="2" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="298"/>
-      <c r="B2" s="298"/>
-      <c r="C2" s="298"/>
-      <c r="D2" s="298"/>
-      <c r="E2" s="298"/>
+      <c r="A2" s="300"/>
+      <c r="B2" s="300"/>
+      <c r="C2" s="300"/>
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="289"/>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289"/>
-      <c r="J2" s="289"/>
-      <c r="K2" s="290"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="292"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="289"/>
-      <c r="N2" s="289"/>
-      <c r="O2" s="289"/>
-      <c r="P2" s="289"/>
-      <c r="Q2" s="290"/>
+      <c r="M2" s="291"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
+      <c r="Q2" s="292"/>
       <c r="R2" s="122"/>
-      <c r="S2" s="289"/>
-      <c r="T2" s="289"/>
-      <c r="U2" s="289"/>
-      <c r="V2" s="289"/>
-      <c r="W2" s="290"/>
+      <c r="S2" s="291"/>
+      <c r="T2" s="291"/>
+      <c r="U2" s="291"/>
+      <c r="V2" s="291"/>
+      <c r="W2" s="292"/>
     </row>
     <row r="3" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -11817,9 +11837,9 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="293"/>
-      <c r="J15" s="293"/>
-      <c r="K15" s="293"/>
+      <c r="I15" s="295"/>
+      <c r="J15" s="295"/>
+      <c r="K15" s="295"/>
       <c r="L15" s="11"/>
       <c r="M15" s="245" t="s">
         <v>362</v>
@@ -11999,13 +12019,13 @@
       <c r="W20" s="11"/>
     </row>
     <row r="21" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="297" t="s">
+      <c r="A21" s="299" t="s">
         <v>356</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -12025,11 +12045,11 @@
       <c r="W21" s="11"/>
     </row>
     <row r="22" spans="1:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -12229,10 +12249,10 @@
         <f>ROUND((B30-60000)*0.48+1400+4225+12180,2)</f>
         <v>27569.02</v>
       </c>
-      <c r="C31" s="302" t="s">
+      <c r="C31" s="304" t="s">
         <v>370</v>
       </c>
-      <c r="D31" s="282"/>
+      <c r="D31" s="284"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -12255,10 +12275,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>420.11</v>
       </c>
-      <c r="C32" s="281" t="s">
+      <c r="C32" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="282"/>
+      <c r="D32" s="284"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -12484,12 +12504,12 @@
         <v>397</v>
       </c>
       <c r="D42" s="11"/>
-      <c r="E42" s="299" t="s">
+      <c r="E42" s="301" t="s">
         <v>375</v>
       </c>
-      <c r="F42" s="300"/>
-      <c r="G42" s="300"/>
-      <c r="H42" s="301"/>
+      <c r="F42" s="302"/>
+      <c r="G42" s="302"/>
+      <c r="H42" s="303"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
@@ -12580,10 +12600,10 @@
       <c r="Q45" s="11"/>
     </row>
     <row r="46" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="277" t="s">
+      <c r="A46" s="279" t="s">
         <v>358</v>
       </c>
-      <c r="B46" s="278"/>
+      <c r="B46" s="280"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
       <c r="E46" s="253" t="s">
@@ -13851,8 +13871,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:B46"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13867,21 +13887,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="297" t="s">
         <v>398</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
       <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="298"/>
-      <c r="B2" s="298"/>
-      <c r="C2" s="298"/>
-      <c r="D2" s="298"/>
-      <c r="E2" s="298"/>
+      <c r="A2" s="300"/>
+      <c r="B2" s="300"/>
+      <c r="C2" s="300"/>
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
       <c r="F2" s="122"/>
     </row>
     <row r="3" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14097,21 +14117,21 @@
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="297" t="s">
+      <c r="A21" s="299" t="s">
         <v>400</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
     </row>
     <row r="22" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
     </row>
     <row r="23" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14212,10 +14232,10 @@
         <f>ROUND((B30-93120)*0.5+32571.75,2)</f>
         <v>34026.410000000003</v>
       </c>
-      <c r="C31" s="302" t="s">
+      <c r="C31" s="304" t="s">
         <v>406</v>
       </c>
-      <c r="D31" s="282"/>
+      <c r="D31" s="284"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
@@ -14227,10 +14247,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>894.01</v>
       </c>
-      <c r="C32" s="281" t="s">
+      <c r="C32" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="282"/>
+      <c r="D32" s="284"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
@@ -14342,22 +14362,22 @@
         <f>B39-B40</f>
         <v>-924.99999999999625</v>
       </c>
-      <c r="C42" s="303" t="s">
+      <c r="C42" s="305" t="s">
         <v>407</v>
       </c>
-      <c r="D42" s="304"/>
-      <c r="E42" s="299" t="s">
+      <c r="D42" s="306"/>
+      <c r="E42" s="301" t="s">
         <v>423</v>
       </c>
-      <c r="F42" s="300"/>
+      <c r="F42" s="302"/>
     </row>
     <row r="43" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="61"/>
       <c r="B43" s="61"/>
-      <c r="C43" s="305" t="s">
+      <c r="C43" s="307" t="s">
         <v>421</v>
       </c>
-      <c r="D43" s="296"/>
+      <c r="D43" s="298"/>
       <c r="E43" s="253" t="s">
         <v>374</v>
       </c>
@@ -14393,10 +14413,10 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="277" t="s">
+      <c r="A46" s="279" t="s">
         <v>426</v>
       </c>
-      <c r="B46" s="278"/>
+      <c r="B46" s="280"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
       <c r="E46" s="253" t="s">
@@ -15641,8 +15661,8 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15659,21 +15679,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="297" t="s">
         <v>424</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
       <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="298"/>
-      <c r="B2" s="298"/>
-      <c r="C2" s="298"/>
-      <c r="D2" s="298"/>
-      <c r="E2" s="298"/>
+      <c r="A2" s="300"/>
+      <c r="B2" s="300"/>
+      <c r="C2" s="300"/>
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
       <c r="F2" s="122"/>
     </row>
     <row r="3" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15889,21 +15909,21 @@
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="297" t="s">
+      <c r="A21" s="299" t="s">
         <v>425</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
     </row>
     <row r="22" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
     </row>
     <row r="23" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16044,10 +16064,10 @@
         <f>ROUND((B33-99266)*0.5+34222.42,2)</f>
         <v>44541.03</v>
       </c>
-      <c r="C34" s="302" t="s">
+      <c r="C34" s="304" t="s">
         <v>406</v>
       </c>
-      <c r="D34" s="282"/>
+      <c r="D34" s="284"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
     </row>
@@ -16059,10 +16079,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>1186.67</v>
       </c>
-      <c r="C35" s="281" t="s">
+      <c r="C35" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="282"/>
+      <c r="D35" s="284"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
     </row>
@@ -16174,20 +16194,22 @@
         <f>B42-B43</f>
         <v>-646.00000000000227</v>
       </c>
-      <c r="C45" s="303" t="s">
+      <c r="C45" s="305" t="s">
         <v>439</v>
       </c>
-      <c r="D45" s="304"/>
-      <c r="E45" s="299" t="s">
+      <c r="D45" s="306"/>
+      <c r="E45" s="301" t="s">
         <v>423</v>
       </c>
-      <c r="F45" s="300"/>
+      <c r="F45" s="302"/>
     </row>
     <row r="46" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="61"/>
       <c r="B46" s="61"/>
-      <c r="C46" s="305"/>
-      <c r="D46" s="296"/>
+      <c r="C46" s="271" t="s">
+        <v>443</v>
+      </c>
+      <c r="D46" s="64"/>
       <c r="E46" s="253" t="s">
         <v>374</v>
       </c>
@@ -16223,10 +16245,10 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="277" t="s">
+      <c r="A49" s="279" t="s">
         <v>426</v>
       </c>
-      <c r="B49" s="278"/>
+      <c r="B49" s="280"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="253" t="s">
@@ -16376,8 +16398,7 @@
       <c r="F56" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C46:D46"/>
+  <mergeCells count="7">
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A21:E22"/>
@@ -16401,7 +16422,7 @@
   </sheetPr>
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -18474,10 +18495,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A104" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18490,11 +18511,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="318" t="s">
+      <c r="A1" s="308" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="320"/>
+      <c r="B1" s="309"/>
+      <c r="C1" s="310"/>
       <c r="D1" s="164"/>
       <c r="E1" s="41" t="s">
         <v>233</v>
@@ -18662,11 +18683,11 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="321" t="s">
+      <c r="A11" s="311" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="322"/>
-      <c r="C11" s="320"/>
+      <c r="B11" s="312"/>
+      <c r="C11" s="310"/>
       <c r="D11" s="164"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -18850,11 +18871,11 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="321" t="s">
+      <c r="A23" s="311" t="s">
         <v>260</v>
       </c>
-      <c r="B23" s="322"/>
-      <c r="C23" s="320"/>
+      <c r="B23" s="312"/>
+      <c r="C23" s="310"/>
       <c r="D23" s="164"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -19130,11 +19151,11 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="323" t="s">
+      <c r="A40" s="313" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="324"/>
-      <c r="C40" s="325"/>
+      <c r="B40" s="314"/>
+      <c r="C40" s="315"/>
       <c r="D40" s="164"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -19226,13 +19247,13 @@
       <c r="C46" s="217">
         <v>-604</v>
       </c>
-      <c r="D46" s="310"/>
-      <c r="E46" s="282"/>
-      <c r="F46" s="282"/>
-      <c r="G46" s="282"/>
-      <c r="H46" s="282"/>
-      <c r="I46" s="282"/>
-      <c r="J46" s="282"/>
+      <c r="D46" s="320"/>
+      <c r="E46" s="284"/>
+      <c r="F46" s="284"/>
+      <c r="G46" s="284"/>
+      <c r="H46" s="284"/>
+      <c r="I46" s="284"/>
+      <c r="J46" s="284"/>
     </row>
     <row r="47" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="180" t="s">
@@ -19366,11 +19387,11 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="311" t="s">
+      <c r="A55" s="321" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="312"/>
-      <c r="C55" s="313"/>
+      <c r="B55" s="322"/>
+      <c r="C55" s="323"/>
       <c r="D55" s="220"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -19681,10 +19702,10 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="314" t="s">
+      <c r="A76" s="324" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="315"/>
+      <c r="B76" s="325"/>
       <c r="C76" s="64"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -19695,8 +19716,8 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="316"/>
-      <c r="B77" s="315"/>
+      <c r="A77" s="326"/>
+      <c r="B77" s="325"/>
       <c r="C77" s="64"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -19735,10 +19756,10 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="306" t="s">
+      <c r="A80" s="316" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="317"/>
+      <c r="B80" s="327"/>
       <c r="C80" s="64"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -19749,8 +19770,8 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="316"/>
-      <c r="B81" s="315"/>
+      <c r="A81" s="326"/>
+      <c r="B81" s="325"/>
       <c r="C81" s="64"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -19957,10 +19978,10 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="306" t="s">
+      <c r="A96" s="316" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="307"/>
+      <c r="B96" s="317"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -19971,8 +19992,8 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="308"/>
-      <c r="B97" s="293"/>
+      <c r="A97" s="318"/>
+      <c r="B97" s="295"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -20121,14 +20142,14 @@
       <c r="B108" s="11"/>
     </row>
     <row r="109" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="309" t="s">
+      <c r="A109" s="319" t="s">
         <v>352</v>
       </c>
-      <c r="B109" s="307"/>
+      <c r="B109" s="317"/>
     </row>
     <row r="110" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="308"/>
-      <c r="B110" s="293"/>
+      <c r="A110" s="318"/>
+      <c r="B110" s="295"/>
     </row>
     <row r="111" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="241" t="s">
@@ -20200,14 +20221,14 @@
       </c>
     </row>
     <row r="124" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="306" t="s">
+      <c r="A124" s="316" t="s">
         <v>416</v>
       </c>
-      <c r="B124" s="307"/>
+      <c r="B124" s="317"/>
     </row>
     <row r="125" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="308"/>
-      <c r="B125" s="293"/>
+      <c r="A125" s="318"/>
+      <c r="B125" s="295"/>
     </row>
     <row r="126" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="230" t="s">
@@ -20225,19 +20246,46 @@
         <v>420</v>
       </c>
     </row>
+    <row r="128" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="316" t="s">
+        <v>440</v>
+      </c>
+      <c r="B128" s="317"/>
+    </row>
+    <row r="129" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="318"/>
+      <c r="B129" s="295"/>
+    </row>
+    <row r="130" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="230" t="s">
+        <v>441</v>
+      </c>
+      <c r="B130" s="270" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="230" t="s">
+        <v>444</v>
+      </c>
+      <c r="B131" s="270" t="s">
+        <v>445</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A96:B97"/>
+  <mergeCells count="12">
+    <mergeCell ref="A128:B129"/>
     <mergeCell ref="A124:B125"/>
     <mergeCell ref="A109:B110"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A76:B77"/>
     <mergeCell ref="A80:B81"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A96:B97"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -21410,20 +21458,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="272" t="s">
+      <c r="A1" s="274" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="274"/>
+      <c r="B1" s="275"/>
+      <c r="C1" s="275"/>
+      <c r="D1" s="275"/>
+      <c r="E1" s="276"/>
     </row>
     <row r="2" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="283"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="285"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="286"/>
+      <c r="C2" s="286"/>
+      <c r="D2" s="286"/>
+      <c r="E2" s="287"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -21583,11 +21631,11 @@
       <c r="B15" s="63">
         <v>438.04</v>
       </c>
-      <c r="C15" s="279" t="s">
+      <c r="C15" s="281" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="280"/>
-      <c r="E15" s="280"/>
+      <c r="D15" s="282"/>
+      <c r="E15" s="282"/>
     </row>
     <row r="16" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -21635,20 +21683,20 @@
       <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="275" t="s">
+      <c r="A21" s="277" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="276"/>
-      <c r="C21" s="276"/>
-      <c r="D21" s="276"/>
-      <c r="E21" s="276"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
     </row>
     <row r="22" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="276"/>
-      <c r="B22" s="276"/>
-      <c r="C22" s="276"/>
-      <c r="D22" s="276"/>
-      <c r="E22" s="276"/>
+      <c r="A22" s="278"/>
+      <c r="B22" s="278"/>
+      <c r="C22" s="278"/>
+      <c r="D22" s="278"/>
+      <c r="E22" s="278"/>
     </row>
     <row r="23" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
@@ -21776,10 +21824,10 @@
         <f>ROUND((B33-18000)*0.35+1750,2)</f>
         <v>5779.41</v>
       </c>
-      <c r="C34" s="281" t="s">
+      <c r="C34" s="283" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="282"/>
+      <c r="D34" s="284"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21790,10 +21838,10 @@
         <f>ROUND((B13-620)*0.06,2)</f>
         <v>244.34</v>
       </c>
-      <c r="C35" s="281" t="s">
+      <c r="C35" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="282"/>
+      <c r="D35" s="284"/>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21920,10 +21968,10 @@
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="277" t="s">
+      <c r="A49" s="279" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="278"/>
+      <c r="B49" s="280"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -25304,34 +25352,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="293" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
+      <c r="B1" s="289"/>
+      <c r="C1" s="289"/>
+      <c r="D1" s="289"/>
+      <c r="E1" s="289"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="286" t="s">
+      <c r="G1" s="288" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="287"/>
-      <c r="K1" s="288"/>
+      <c r="H1" s="289"/>
+      <c r="I1" s="289"/>
+      <c r="J1" s="289"/>
+      <c r="K1" s="290"/>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="283"/>
-      <c r="B2" s="289"/>
-      <c r="C2" s="289"/>
-      <c r="D2" s="289"/>
-      <c r="E2" s="289"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="291"/>
+      <c r="C2" s="291"/>
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="289"/>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289"/>
-      <c r="J2" s="289"/>
-      <c r="K2" s="290"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="292"/>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -25630,11 +25678,11 @@
       <c r="B15" s="63">
         <v>1535.69</v>
       </c>
-      <c r="C15" s="279" t="s">
+      <c r="C15" s="281" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="280"/>
-      <c r="E15" s="280"/>
+      <c r="D15" s="282"/>
+      <c r="E15" s="282"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -25642,11 +25690,11 @@
       <c r="H15" s="63">
         <v>413.13</v>
       </c>
-      <c r="I15" s="279" t="s">
+      <c r="I15" s="281" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="280"/>
-      <c r="K15" s="280"/>
+      <c r="J15" s="282"/>
+      <c r="K15" s="282"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -25734,13 +25782,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="275" t="s">
+      <c r="A21" s="277" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -25749,11 +25797,11 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -25954,10 +26002,10 @@
         <f>ROUND((B33-31000)*0.42+6300,2)</f>
         <v>7196.73</v>
       </c>
-      <c r="C34" s="281" t="s">
+      <c r="C34" s="283" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="282"/>
+      <c r="D34" s="284"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -25974,10 +26022,10 @@
         <f>ROUND((B13+H13-620)*0.06,2)</f>
         <v>312.08999999999997</v>
       </c>
-      <c r="C35" s="281" t="s">
+      <c r="C35" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="282"/>
+      <c r="D35" s="284"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -26201,10 +26249,10 @@
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="277" t="s">
+      <c r="A50" s="279" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="278"/>
+      <c r="B50" s="280"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -29976,48 +30024,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="293" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
+      <c r="B1" s="289"/>
+      <c r="C1" s="289"/>
+      <c r="D1" s="289"/>
+      <c r="E1" s="289"/>
       <c r="F1" s="122"/>
-      <c r="G1" s="286" t="s">
+      <c r="G1" s="288" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="287"/>
-      <c r="K1" s="287"/>
+      <c r="H1" s="289"/>
+      <c r="I1" s="289"/>
+      <c r="J1" s="289"/>
+      <c r="K1" s="289"/>
       <c r="L1" s="122"/>
-      <c r="M1" s="286" t="s">
+      <c r="M1" s="288" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="287"/>
-      <c r="O1" s="287"/>
-      <c r="P1" s="287"/>
-      <c r="Q1" s="288"/>
+      <c r="N1" s="289"/>
+      <c r="O1" s="289"/>
+      <c r="P1" s="289"/>
+      <c r="Q1" s="290"/>
     </row>
     <row r="2" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="283"/>
-      <c r="B2" s="289"/>
-      <c r="C2" s="289"/>
-      <c r="D2" s="289"/>
-      <c r="E2" s="289"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="291"/>
+      <c r="C2" s="291"/>
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
       <c r="F2" s="122"/>
-      <c r="G2" s="289"/>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289"/>
-      <c r="J2" s="289"/>
-      <c r="K2" s="289"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="291"/>
       <c r="L2" s="122"/>
-      <c r="M2" s="289"/>
-      <c r="N2" s="289"/>
-      <c r="O2" s="289"/>
-      <c r="P2" s="289"/>
-      <c r="Q2" s="290"/>
+      <c r="M2" s="291"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
+      <c r="Q2" s="292"/>
     </row>
     <row r="3" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
@@ -30455,11 +30503,11 @@
       <c r="B15" s="63">
         <v>175.89</v>
       </c>
-      <c r="C15" s="279" t="s">
+      <c r="C15" s="281" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="280"/>
-      <c r="E15" s="280"/>
+      <c r="D15" s="282"/>
+      <c r="E15" s="282"/>
       <c r="F15" s="123"/>
       <c r="G15" s="127" t="s">
         <v>90</v>
@@ -30467,17 +30515,17 @@
       <c r="H15" s="63">
         <v>13.93</v>
       </c>
-      <c r="I15" s="279" t="s">
+      <c r="I15" s="281" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="280"/>
-      <c r="K15" s="280"/>
+      <c r="J15" s="282"/>
+      <c r="K15" s="282"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="293"/>
-      <c r="P15" s="293"/>
-      <c r="Q15" s="293"/>
+      <c r="O15" s="295"/>
+      <c r="P15" s="295"/>
+      <c r="Q15" s="295"/>
     </row>
     <row r="16" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="62" t="s">
@@ -30601,13 +30649,13 @@
       <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="275" t="s">
+      <c r="A21" s="277" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
+      <c r="B21" s="294"/>
+      <c r="C21" s="294"/>
+      <c r="D21" s="294"/>
+      <c r="E21" s="294"/>
       <c r="F21" s="76"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -30622,11 +30670,11 @@
       <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="292"/>
-      <c r="D22" s="292"/>
-      <c r="E22" s="292"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="294"/>
+      <c r="C22" s="294"/>
+      <c r="D22" s="294"/>
+      <c r="E22" s="294"/>
       <c r="F22" s="76"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -30875,10 +30923,10 @@
         <f>ROUND((B32-31000)*0.42+6300,2)</f>
         <v>8538.18</v>
       </c>
-      <c r="C33" s="281" t="s">
+      <c r="C33" s="283" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="282"/>
+      <c r="D33" s="284"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -30901,10 +30949,10 @@
         <f>ROUND((B13+H13+N13-620)*0.06,2)</f>
         <v>329.36</v>
       </c>
-      <c r="C34" s="281" t="s">
+      <c r="C34" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="282"/>
+      <c r="D34" s="284"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -31182,10 +31230,10 @@
       <c r="Q46" s="11"/>
     </row>
     <row r="47" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="277" t="s">
+      <c r="A47" s="279" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="278"/>
+      <c r="B47" s="280"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>

</xml_diff>